<commit_message>
adição da Mobilidade Elétrica, no arquivo xlsx e no arquivo .py
</commit_message>
<xml_diff>
--- a/kpis_energia_por_unidade.xlsx
+++ b/kpis_energia_por_unidade.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f78391ab5a1cfb12/01 - NASCIMENTO/CEAMAZON/ProjKpi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayrton\Documents\GitHub\atnee\kpis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="14_{654616FC-0284-4458-954F-BCECCAE4DE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E88A77FE-7AC7-4644-A109-2CE153F3F7E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E348873E-9A59-44DB-AA1D-5F6377E5BF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23610" yWindow="525" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rodoviário" sheetId="2" r:id="rId2"/>
+    <sheet name="Urbano" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>-</t>
   </si>
@@ -79,20 +81,73 @@
   <si>
     <t>Tempo</t>
   </si>
+  <si>
+    <t>Mês</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>Dias</t>
+  </si>
+  <si>
+    <t>Preço Diesel s10 (R$/L)</t>
+  </si>
+  <si>
+    <t>Coefiente de GEE</t>
+  </si>
+  <si>
+    <t>Litros (Combustão)</t>
+  </si>
+  <si>
+    <t>Litros de Diesel</t>
+  </si>
+  <si>
+    <t>Emissão de GEE (Elétrico) (kg CO2)</t>
+  </si>
+  <si>
+    <t>Coeficiente de Emissão Combustão</t>
+  </si>
+  <si>
+    <t>Emissão de GEE (Diesel) (kgCO2)</t>
+  </si>
+  <si>
+    <t>Redução da Emissão</t>
+  </si>
+  <si>
+    <t>Percentual de Redução</t>
+  </si>
+  <si>
+    <t>Gasto em Diesel</t>
+  </si>
+  <si>
+    <t>Tarifa Fora Ponta</t>
+  </si>
+  <si>
+    <t>Gasto em Energia Elétrica</t>
+  </si>
+  <si>
+    <t>Economia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-416]mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
+    <numFmt numFmtId="169" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +199,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +238,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,14 +253,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -266,10 +367,68 @@
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Moeda" xfId="3" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="4" builtinId="5"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
     <cellStyle name="Vírgula 4" xfId="2" xr:uid="{7CBFA859-85D8-46D5-A762-F87CB82252FC}"/>
   </cellStyles>
@@ -551,7 +710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14:L49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2622,4 +2783,4582 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AC82A9-1A92-44C2-9406-62A85459B06F}">
+  <dimension ref="A1:Q41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="40">
+        <v>44562</v>
+      </c>
+      <c r="B2" s="41">
+        <v>2652.18</v>
+      </c>
+      <c r="C2" s="41">
+        <v>2886.84</v>
+      </c>
+      <c r="D2" s="41">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E37" si="0">(B2/P2)*N2</f>
+        <v>2843.1369599999998</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F37" si="1">B2*O2</f>
+        <v>194.13957600000001</v>
+      </c>
+      <c r="G2">
+        <f>(E2-F2)/1000</f>
+        <v>2.6489973839999998</v>
+      </c>
+      <c r="H2" s="53">
+        <f>((E2-F2)/E2)*100</f>
+        <v>93.171641791044777</v>
+      </c>
+      <c r="I2" s="30">
+        <f t="shared" ref="I2:I37" si="2">B2/P2</f>
+        <v>1060.8719999999998</v>
+      </c>
+      <c r="J2" s="48">
+        <f>I2*Q2</f>
+        <v>5824.1872799999992</v>
+      </c>
+      <c r="K2" s="48">
+        <f>C2*M2</f>
+        <v>1159.56857016</v>
+      </c>
+      <c r="L2" s="48">
+        <f>J2-K2</f>
+        <v>4664.6187098399987</v>
+      </c>
+      <c r="M2" s="21">
+        <v>0.40167399999999998</v>
+      </c>
+      <c r="N2">
+        <v>2.68</v>
+      </c>
+      <c r="O2" s="28">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="P2" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q2" s="43">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="40">
+        <v>44593</v>
+      </c>
+      <c r="B3" s="41">
+        <v>601.24</v>
+      </c>
+      <c r="C3" s="41">
+        <v>628.55999999999995</v>
+      </c>
+      <c r="D3" s="41">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>644.52928000000009</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>30.214739543725244</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G37" si="3">(E3-F3)/1000</f>
+        <v>0.61431454045627476</v>
+      </c>
+      <c r="H3" s="53">
+        <f t="shared" ref="H3:H37" si="4">((E3-F3)/E3)*100</f>
+        <v>95.31212305145776</v>
+      </c>
+      <c r="I3" s="30">
+        <f t="shared" si="2"/>
+        <v>240.49600000000001</v>
+      </c>
+      <c r="J3" s="48">
+        <f t="shared" ref="J3:J37" si="5">I3*Q3</f>
+        <v>1346.7775999999999</v>
+      </c>
+      <c r="K3" s="48">
+        <f t="shared" ref="K3:K37" si="6">C3*M3</f>
+        <v>259.59590856</v>
+      </c>
+      <c r="L3" s="48">
+        <f t="shared" ref="L3:L37" si="7">J3-K3</f>
+        <v>1087.1816914399999</v>
+      </c>
+      <c r="M3" s="21">
+        <v>0.41300100000000001</v>
+      </c>
+      <c r="N3">
+        <v>2.68</v>
+      </c>
+      <c r="O3" s="28">
+        <v>5.0254040888372771E-2</v>
+      </c>
+      <c r="P3" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q3" s="43">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="40">
+        <v>44621</v>
+      </c>
+      <c r="B4" s="41">
+        <v>3128.78</v>
+      </c>
+      <c r="C4" s="41">
+        <v>3657.96</v>
+      </c>
+      <c r="D4" s="41">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>3354.0521600000006</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>127.07585412700854</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>3.2269763058729923</v>
+      </c>
+      <c r="H4" s="53">
+        <f t="shared" si="4"/>
+        <v>96.211273764835894</v>
+      </c>
+      <c r="I4" s="30">
+        <f t="shared" si="2"/>
+        <v>1251.5120000000002</v>
+      </c>
+      <c r="J4" s="48">
+        <f t="shared" si="5"/>
+        <v>7846.9802400000008</v>
+      </c>
+      <c r="K4" s="48">
+        <f t="shared" si="6"/>
+        <v>1466.5310334000001</v>
+      </c>
+      <c r="L4" s="48">
+        <f t="shared" si="7"/>
+        <v>6380.4492066000003</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0.40091500000000002</v>
+      </c>
+      <c r="N4">
+        <v>2.68</v>
+      </c>
+      <c r="O4" s="28">
+        <v>4.0615145240959265E-2</v>
+      </c>
+      <c r="P4" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q4" s="43">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="40">
+        <v>44652</v>
+      </c>
+      <c r="B5" s="41">
+        <v>2418</v>
+      </c>
+      <c r="C5" s="41">
+        <v>3116.88</v>
+      </c>
+      <c r="D5" s="41">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2592.0960000000005</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>52.20013493737396</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>2.5398958650626264</v>
+      </c>
+      <c r="H5" s="53">
+        <f t="shared" si="4"/>
+        <v>97.986180491101635</v>
+      </c>
+      <c r="I5" s="30">
+        <f t="shared" si="2"/>
+        <v>967.2</v>
+      </c>
+      <c r="J5" s="48">
+        <f t="shared" si="5"/>
+        <v>6393.1920000000009</v>
+      </c>
+      <c r="K5" s="48">
+        <f t="shared" si="6"/>
+        <v>1273.1083372799999</v>
+      </c>
+      <c r="L5" s="48">
+        <f t="shared" si="7"/>
+        <v>5120.0836627200006</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0.40845599999999999</v>
+      </c>
+      <c r="N5">
+        <v>2.68</v>
+      </c>
+      <c r="O5" s="28">
+        <v>2.1588145135390389E-2</v>
+      </c>
+      <c r="P5" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q5" s="43">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="40">
+        <v>44682</v>
+      </c>
+      <c r="B6" s="41">
+        <v>3318.2</v>
+      </c>
+      <c r="C6" s="41">
+        <v>4147.2</v>
+      </c>
+      <c r="D6" s="41">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3557.1104</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>92.993311139522831</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>3.4641170888604771</v>
+      </c>
+      <c r="H6" s="53">
+        <f t="shared" si="4"/>
+        <v>97.385706354811958</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" si="2"/>
+        <v>1327.28</v>
+      </c>
+      <c r="J6" s="48">
+        <f t="shared" si="5"/>
+        <v>9105.140800000001</v>
+      </c>
+      <c r="K6" s="48">
+        <f t="shared" si="6"/>
+        <v>1718.9356031999998</v>
+      </c>
+      <c r="L6" s="48">
+        <f t="shared" si="7"/>
+        <v>7386.2051968000014</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0.41448099999999999</v>
+      </c>
+      <c r="N6">
+        <v>2.68</v>
+      </c>
+      <c r="O6" s="28">
+        <v>2.8025227876415777E-2</v>
+      </c>
+      <c r="P6" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q6" s="43">
+        <v>6.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="40">
+        <v>44713</v>
+      </c>
+      <c r="B7" s="41">
+        <v>3167.37</v>
+      </c>
+      <c r="C7" s="41">
+        <v>3962.52</v>
+      </c>
+      <c r="D7" s="41">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3395.4206399999998</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>139.55623849164192</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>3.255864401508358</v>
+      </c>
+      <c r="H7" s="53">
+        <f t="shared" si="4"/>
+        <v>95.889868935601399</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" si="2"/>
+        <v>1266.9479999999999</v>
+      </c>
+      <c r="J7" s="48">
+        <f t="shared" si="5"/>
+        <v>9122.025599999999</v>
+      </c>
+      <c r="K7" s="48">
+        <f t="shared" si="6"/>
+        <v>1623.02441688</v>
+      </c>
+      <c r="L7" s="48">
+        <f t="shared" si="7"/>
+        <v>7499.001183119999</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0.40959400000000001</v>
+      </c>
+      <c r="N7">
+        <v>2.68</v>
+      </c>
+      <c r="O7" s="28">
+        <v>4.4060605010353047E-2</v>
+      </c>
+      <c r="P7" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q7" s="43">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
+        <v>44743</v>
+      </c>
+      <c r="B8" s="41">
+        <v>2977.96</v>
+      </c>
+      <c r="C8" s="41">
+        <v>3508.92</v>
+      </c>
+      <c r="D8" s="41">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>3192.3731200000002</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>124.67446157965476</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>3.0676986584203454</v>
+      </c>
+      <c r="H8" s="53">
+        <f t="shared" si="4"/>
+        <v>96.094614980981461</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="shared" si="2"/>
+        <v>1191.184</v>
+      </c>
+      <c r="J8" s="48">
+        <f t="shared" si="5"/>
+        <v>8850.49712</v>
+      </c>
+      <c r="K8" s="48">
+        <f t="shared" si="6"/>
+        <v>1319.0732063999999</v>
+      </c>
+      <c r="L8" s="48">
+        <f t="shared" si="7"/>
+        <v>7531.4239135999997</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.37591999999999998</v>
+      </c>
+      <c r="N8">
+        <v>2.68</v>
+      </c>
+      <c r="O8" s="28">
+        <v>4.1865727403878748E-2</v>
+      </c>
+      <c r="P8" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q8" s="43">
+        <v>7.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>44774</v>
+      </c>
+      <c r="B9" s="41">
+        <v>2991.78</v>
+      </c>
+      <c r="C9" s="41">
+        <v>3926.88</v>
+      </c>
+      <c r="D9" s="41">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3207.1881600000002</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>136.76646388475945</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>3.0704216961152406</v>
+      </c>
+      <c r="H9" s="53">
+        <f t="shared" si="4"/>
+        <v>95.735627064526213</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="2"/>
+        <v>1196.712</v>
+      </c>
+      <c r="J9" s="48">
+        <f t="shared" si="5"/>
+        <v>8484.6880799999999</v>
+      </c>
+      <c r="K9" s="48">
+        <f t="shared" si="6"/>
+        <v>1620.8236468800001</v>
+      </c>
+      <c r="L9" s="48">
+        <f t="shared" si="7"/>
+        <v>6863.8644331199994</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0.41275099999999998</v>
+      </c>
+      <c r="N9">
+        <v>2.68</v>
+      </c>
+      <c r="O9" s="28">
+        <v>4.5714077868278892E-2</v>
+      </c>
+      <c r="P9" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q9" s="43">
+        <v>7.09</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="40">
+        <v>44805</v>
+      </c>
+      <c r="B10" s="41">
+        <v>3177.56</v>
+      </c>
+      <c r="C10" s="41">
+        <v>4228.2</v>
+      </c>
+      <c r="D10" s="41">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3406.3443199999997</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>155.97561569625259</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>3.2503687043037472</v>
+      </c>
+      <c r="H10" s="53">
+        <f t="shared" si="4"/>
+        <v>95.421026148752546</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="2"/>
+        <v>1271.0239999999999</v>
+      </c>
+      <c r="J10" s="48">
+        <f t="shared" si="5"/>
+        <v>8693.8041599999997</v>
+      </c>
+      <c r="K10" s="48">
+        <f t="shared" si="6"/>
+        <v>1758.4111313999999</v>
+      </c>
+      <c r="L10" s="48">
+        <f t="shared" si="7"/>
+        <v>6935.3930285999995</v>
+      </c>
+      <c r="M10" s="21">
+        <v>0.415877</v>
+      </c>
+      <c r="N10">
+        <v>2.68</v>
+      </c>
+      <c r="O10" s="28">
+        <v>4.9086599685372614E-2</v>
+      </c>
+      <c r="P10" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q10" s="43">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
+        <v>44835</v>
+      </c>
+      <c r="B11" s="41">
+        <v>2560.7199999999998</v>
+      </c>
+      <c r="C11" s="41">
+        <v>3593.16</v>
+      </c>
+      <c r="D11" s="41">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2745.09184</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>120.67423813055775</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>2.6244176018694425</v>
+      </c>
+      <c r="H11" s="53">
+        <f t="shared" si="4"/>
+        <v>95.603999969248477</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" si="2"/>
+        <v>1024.288</v>
+      </c>
+      <c r="J11" s="48">
+        <f t="shared" si="5"/>
+        <v>6627.14336</v>
+      </c>
+      <c r="K11" s="48">
+        <f t="shared" si="6"/>
+        <v>1486.1094170399999</v>
+      </c>
+      <c r="L11" s="48">
+        <f t="shared" si="7"/>
+        <v>5141.0339429599999</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0.41359400000000002</v>
+      </c>
+      <c r="N11">
+        <v>2.68</v>
+      </c>
+      <c r="O11" s="28">
+        <v>4.7125120329656413E-2</v>
+      </c>
+      <c r="P11" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q11" s="43">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="40">
+        <v>44866</v>
+      </c>
+      <c r="B12" s="41">
+        <v>2304.3200000000002</v>
+      </c>
+      <c r="C12" s="41">
+        <v>2928.96</v>
+      </c>
+      <c r="D12" s="41">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2470.2310400000001</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>92.733691531719629</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>2.3774973484682804</v>
+      </c>
+      <c r="H12" s="53">
+        <f t="shared" si="4"/>
+        <v>96.245950681126587</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="2"/>
+        <v>921.72800000000007</v>
+      </c>
+      <c r="J12" s="48">
+        <f t="shared" si="5"/>
+        <v>5991.232</v>
+      </c>
+      <c r="K12" s="48">
+        <f t="shared" si="6"/>
+        <v>1204.1598931199999</v>
+      </c>
+      <c r="L12" s="48">
+        <f t="shared" si="7"/>
+        <v>4787.0721068800003</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0.41112199999999999</v>
+      </c>
+      <c r="N12">
+        <v>2.68</v>
+      </c>
+      <c r="O12" s="28">
+        <v>4.0243408698322984E-2</v>
+      </c>
+      <c r="P12" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q12" s="43">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="40">
+        <v>44896</v>
+      </c>
+      <c r="B13" s="41">
+        <v>0</v>
+      </c>
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="41">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0.41761399999999999</v>
+      </c>
+      <c r="N13">
+        <v>2.68</v>
+      </c>
+      <c r="O13" s="28">
+        <v>2.9368484258302584E-2</v>
+      </c>
+      <c r="P13" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q13" s="43">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="40">
+        <v>44927</v>
+      </c>
+      <c r="B14" s="41">
+        <v>0</v>
+      </c>
+      <c r="C14" s="41">
+        <v>0</v>
+      </c>
+      <c r="D14" s="41">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="22">
+        <v>0.41628599999999999</v>
+      </c>
+      <c r="N14">
+        <v>2.68</v>
+      </c>
+      <c r="O14" s="28">
+        <v>2.9173607327091757E-2</v>
+      </c>
+      <c r="P14" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q14" s="43">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="40">
+        <v>44958</v>
+      </c>
+      <c r="B15" s="41">
+        <v>1013.4349999999977</v>
+      </c>
+      <c r="C15" s="41">
+        <v>774.36</v>
+      </c>
+      <c r="D15" s="41">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1086.4023199999976</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>24.093174996317973</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>1.0623091450036797</v>
+      </c>
+      <c r="H15" s="53">
+        <f t="shared" si="4"/>
+        <v>97.782297169954688</v>
+      </c>
+      <c r="I15" s="30">
+        <f t="shared" si="2"/>
+        <v>405.37399999999906</v>
+      </c>
+      <c r="J15" s="48">
+        <f t="shared" si="5"/>
+        <v>2456.5664399999941</v>
+      </c>
+      <c r="K15" s="48">
+        <f t="shared" si="6"/>
+        <v>329.36473368000003</v>
+      </c>
+      <c r="L15" s="48">
+        <f t="shared" si="7"/>
+        <v>2127.2017063199942</v>
+      </c>
+      <c r="M15" s="22">
+        <v>0.42533799999999999</v>
+      </c>
+      <c r="N15">
+        <v>2.68</v>
+      </c>
+      <c r="O15" s="28">
+        <v>2.3773774338085845E-2</v>
+      </c>
+      <c r="P15" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q15" s="43">
+        <v>6.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="40">
+        <v>44986</v>
+      </c>
+      <c r="B16" s="41">
+        <v>272</v>
+      </c>
+      <c r="C16" s="41">
+        <v>463.32</v>
+      </c>
+      <c r="D16" s="41">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>291.584</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>8.0438485278792147</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>0.2835401514721208</v>
+      </c>
+      <c r="H16" s="53">
+        <f t="shared" si="4"/>
+        <v>97.24132718946197</v>
+      </c>
+      <c r="I16" s="30">
+        <f t="shared" si="2"/>
+        <v>108.8</v>
+      </c>
+      <c r="J16" s="48">
+        <f t="shared" si="5"/>
+        <v>638.65599999999995</v>
+      </c>
+      <c r="K16" s="48">
+        <f t="shared" si="6"/>
+        <v>198.13462812</v>
+      </c>
+      <c r="L16" s="48">
+        <f t="shared" si="7"/>
+        <v>440.52137187999995</v>
+      </c>
+      <c r="M16" s="22">
+        <v>0.42764099999999999</v>
+      </c>
+      <c r="N16">
+        <v>2.68</v>
+      </c>
+      <c r="O16" s="28">
+        <v>2.9572972528967699E-2</v>
+      </c>
+      <c r="P16" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q16" s="43">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="40">
+        <v>45017</v>
+      </c>
+      <c r="B17" s="41">
+        <v>0</v>
+      </c>
+      <c r="C17" s="41">
+        <v>0</v>
+      </c>
+      <c r="D17" s="41">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="22">
+        <v>0.41775099999999998</v>
+      </c>
+      <c r="N17">
+        <v>2.68</v>
+      </c>
+      <c r="O17" s="28">
+        <v>3.40267536628742E-2</v>
+      </c>
+      <c r="P17" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q17" s="43">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="40">
+        <v>45047</v>
+      </c>
+      <c r="B18" s="41">
+        <v>147</v>
+      </c>
+      <c r="C18" s="41">
+        <v>142.56</v>
+      </c>
+      <c r="D18" s="41">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>157.584</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>4.3380851129783684</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>0.15324591488702163</v>
+      </c>
+      <c r="H18" s="53">
+        <f t="shared" si="4"/>
+        <v>97.24712844389127</v>
+      </c>
+      <c r="I18" s="30">
+        <f t="shared" si="2"/>
+        <v>58.8</v>
+      </c>
+      <c r="J18" s="48">
+        <f t="shared" si="5"/>
+        <v>316.34399999999999</v>
+      </c>
+      <c r="K18" s="48">
+        <f t="shared" si="6"/>
+        <v>59.961021119999998</v>
+      </c>
+      <c r="L18" s="48">
+        <f t="shared" si="7"/>
+        <v>256.38297888</v>
+      </c>
+      <c r="M18" s="22">
+        <v>0.42060199999999998</v>
+      </c>
+      <c r="N18">
+        <v>2.68</v>
+      </c>
+      <c r="O18" s="28">
+        <v>2.9510783081485501E-2</v>
+      </c>
+      <c r="P18" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q18" s="43">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="40">
+        <v>45078</v>
+      </c>
+      <c r="B19" s="41">
+        <v>0</v>
+      </c>
+      <c r="C19" s="41">
+        <v>0</v>
+      </c>
+      <c r="D19" s="41">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="22">
+        <v>0.426981</v>
+      </c>
+      <c r="N19">
+        <v>2.68</v>
+      </c>
+      <c r="O19" s="28">
+        <v>5.2787803573402799E-2</v>
+      </c>
+      <c r="P19" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q19" s="43">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="40">
+        <v>45108</v>
+      </c>
+      <c r="B20" s="41">
+        <v>0</v>
+      </c>
+      <c r="C20" s="41">
+        <v>0</v>
+      </c>
+      <c r="D20" s="41">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="22">
+        <v>0.43435200000000002</v>
+      </c>
+      <c r="N20">
+        <v>2.68</v>
+      </c>
+      <c r="O20" s="28">
+        <v>4.9510010162503372E-2</v>
+      </c>
+      <c r="P20" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q20" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="40">
+        <v>45139</v>
+      </c>
+      <c r="B21" s="41">
+        <v>162</v>
+      </c>
+      <c r="C21" s="41">
+        <v>142.55999999999995</v>
+      </c>
+      <c r="D21" s="41">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>173.66400000000002</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>6.7879404668909711</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.16687605953310905</v>
+      </c>
+      <c r="H21" s="53">
+        <f t="shared" si="4"/>
+        <v>96.091337026159152</v>
+      </c>
+      <c r="I21" s="30">
+        <f t="shared" si="2"/>
+        <v>64.8</v>
+      </c>
+      <c r="J21" s="48">
+        <f t="shared" si="5"/>
+        <v>358.34399999999999</v>
+      </c>
+      <c r="K21" s="48">
+        <f t="shared" si="6"/>
+        <v>70.359062399999971</v>
+      </c>
+      <c r="L21" s="48">
+        <f t="shared" si="7"/>
+        <v>287.98493760000002</v>
+      </c>
+      <c r="M21" s="22">
+        <v>0.49353999999999998</v>
+      </c>
+      <c r="N21">
+        <v>2.68</v>
+      </c>
+      <c r="O21" s="28">
+        <v>4.1900867079573897E-2</v>
+      </c>
+      <c r="P21" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q21" s="43">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="40">
+        <v>45170</v>
+      </c>
+      <c r="B22" s="41">
+        <v>0</v>
+      </c>
+      <c r="C22" s="41">
+        <v>0</v>
+      </c>
+      <c r="D22" s="41">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="22">
+        <v>0.55518699999999999</v>
+      </c>
+      <c r="N22">
+        <v>2.68</v>
+      </c>
+      <c r="O22" s="28">
+        <v>3.4334475892947448E-2</v>
+      </c>
+      <c r="P22" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q22" s="43">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="40">
+        <v>45200</v>
+      </c>
+      <c r="B23" s="41">
+        <v>0</v>
+      </c>
+      <c r="C23" s="41">
+        <v>0</v>
+      </c>
+      <c r="D23" s="41">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="22">
+        <v>0.53955500000000001</v>
+      </c>
+      <c r="N23">
+        <v>2.68</v>
+      </c>
+      <c r="O23" s="28">
+        <v>3.8729598739869808E-2</v>
+      </c>
+      <c r="P23" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q23" s="43">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="40">
+        <v>45231</v>
+      </c>
+      <c r="B24" s="41">
+        <v>63</v>
+      </c>
+      <c r="C24" s="41">
+        <v>90</v>
+      </c>
+      <c r="D24" s="41">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>67.536000000000001</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>3.3343173603629235</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>6.4201682639637089E-2</v>
+      </c>
+      <c r="H24" s="53">
+        <f t="shared" si="4"/>
+        <v>95.062903695269313</v>
+      </c>
+      <c r="I24" s="30">
+        <f t="shared" si="2"/>
+        <v>25.2</v>
+      </c>
+      <c r="J24" s="48">
+        <f t="shared" si="5"/>
+        <v>153.21600000000001</v>
+      </c>
+      <c r="K24" s="48">
+        <f t="shared" si="6"/>
+        <v>48.633030000000005</v>
+      </c>
+      <c r="L24" s="48">
+        <f t="shared" si="7"/>
+        <v>104.58297</v>
+      </c>
+      <c r="M24" s="22">
+        <v>0.54036700000000004</v>
+      </c>
+      <c r="N24">
+        <v>2.68</v>
+      </c>
+      <c r="O24" s="28">
+        <v>5.2925672386713071E-2</v>
+      </c>
+      <c r="P24" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q24" s="43">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="40">
+        <v>45261</v>
+      </c>
+      <c r="B25" s="41">
+        <v>0</v>
+      </c>
+      <c r="C25" s="41">
+        <v>0</v>
+      </c>
+      <c r="D25" s="41">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="23">
+        <v>0.54342199999999996</v>
+      </c>
+      <c r="N25">
+        <v>2.68</v>
+      </c>
+      <c r="O25" s="28">
+        <v>4.586845854173565E-2</v>
+      </c>
+      <c r="P25" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q25" s="43">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="40">
+        <v>45292</v>
+      </c>
+      <c r="B26" s="42">
+        <v>1260</v>
+      </c>
+      <c r="C26" s="41">
+        <v>1487.16</v>
+      </c>
+      <c r="D26" s="41">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1350.72</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>53.046185029783345</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>1.2976738149702167</v>
+      </c>
+      <c r="H26" s="53">
+        <f t="shared" si="4"/>
+        <v>96.072747495425887</v>
+      </c>
+      <c r="I26" s="30">
+        <f t="shared" si="2"/>
+        <v>504</v>
+      </c>
+      <c r="J26" s="48">
+        <f t="shared" si="5"/>
+        <v>2963.52</v>
+      </c>
+      <c r="K26" s="48">
+        <f t="shared" si="6"/>
+        <v>814.69004256000005</v>
+      </c>
+      <c r="L26" s="48">
+        <f t="shared" si="7"/>
+        <v>2148.8299574399998</v>
+      </c>
+      <c r="M26" s="22">
+        <v>0.54781599999999997</v>
+      </c>
+      <c r="N26">
+        <v>2.68</v>
+      </c>
+      <c r="O26" s="28">
+        <v>4.2100146849034403E-2</v>
+      </c>
+      <c r="P26" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q26" s="43">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="40">
+        <v>45323</v>
+      </c>
+      <c r="B27" s="41">
+        <v>213</v>
+      </c>
+      <c r="C27" s="41">
+        <v>249.48</v>
+      </c>
+      <c r="D27" s="41">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>228.33600000000001</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>8.0037203934103633</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>0.22033227960658966</v>
+      </c>
+      <c r="H27" s="53">
+        <f t="shared" si="4"/>
+        <v>96.494761932673626</v>
+      </c>
+      <c r="I27" s="30">
+        <f t="shared" si="2"/>
+        <v>85.2</v>
+      </c>
+      <c r="J27" s="48">
+        <f t="shared" si="5"/>
+        <v>500.976</v>
+      </c>
+      <c r="K27" s="48">
+        <f t="shared" si="6"/>
+        <v>137.41034076</v>
+      </c>
+      <c r="L27" s="48">
+        <f t="shared" si="7"/>
+        <v>363.56565924</v>
+      </c>
+      <c r="M27" s="22">
+        <v>0.55078700000000003</v>
+      </c>
+      <c r="N27">
+        <v>2.68</v>
+      </c>
+      <c r="O27" s="28">
+        <v>3.7576152081738791E-2</v>
+      </c>
+      <c r="P27" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q27" s="43">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="40">
+        <v>45352</v>
+      </c>
+      <c r="B28" s="41">
+        <v>0</v>
+      </c>
+      <c r="C28" s="41">
+        <v>0</v>
+      </c>
+      <c r="D28" s="41">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="23">
+        <v>0.546991</v>
+      </c>
+      <c r="N28">
+        <v>2.68</v>
+      </c>
+      <c r="O28" s="28">
+        <v>2.7790975910056099E-2</v>
+      </c>
+      <c r="P28" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q28" s="43">
+        <v>5.1933031268038796</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="40">
+        <v>45383</v>
+      </c>
+      <c r="B29" s="41">
+        <v>0</v>
+      </c>
+      <c r="C29" s="41">
+        <v>0</v>
+      </c>
+      <c r="D29" s="41">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="23">
+        <v>0.53952599999999995</v>
+      </c>
+      <c r="N29">
+        <v>2.68</v>
+      </c>
+      <c r="O29" s="28">
+        <v>1.9463441675685741E-2</v>
+      </c>
+      <c r="P29" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q29" s="43">
+        <v>5.8975999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="40">
+        <v>45413</v>
+      </c>
+      <c r="B30" s="41">
+        <v>113</v>
+      </c>
+      <c r="C30" s="41">
+        <v>161.99999999999997</v>
+      </c>
+      <c r="D30" s="41">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>121.13600000000001</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>3.2027243083068129</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>0.11793327569169319</v>
+      </c>
+      <c r="H30" s="53">
+        <f t="shared" si="4"/>
+        <v>97.356092071467756</v>
+      </c>
+      <c r="I30" s="30">
+        <f t="shared" si="2"/>
+        <v>45.2</v>
+      </c>
+      <c r="J30" s="48">
+        <f t="shared" si="5"/>
+        <v>266.88567723369965</v>
+      </c>
+      <c r="K30" s="48">
+        <f t="shared" si="6"/>
+        <v>88.412471999999994</v>
+      </c>
+      <c r="L30" s="48">
+        <f t="shared" si="7"/>
+        <v>178.47320523369967</v>
+      </c>
+      <c r="M30" s="23">
+        <v>0.54575600000000002</v>
+      </c>
+      <c r="N30">
+        <v>2.68</v>
+      </c>
+      <c r="O30" s="28">
+        <v>2.83426929938656E-2</v>
+      </c>
+      <c r="P30" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q30" s="43">
+        <v>5.9045503812765405</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
+        <v>45444</v>
+      </c>
+      <c r="B31" s="41">
+        <v>0</v>
+      </c>
+      <c r="C31" s="41">
+        <v>0</v>
+      </c>
+      <c r="D31" s="41">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="23">
+        <v>0.556674</v>
+      </c>
+      <c r="N31">
+        <v>2.68</v>
+      </c>
+      <c r="O31" s="28">
+        <v>3.6478268557543055E-2</v>
+      </c>
+      <c r="P31" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q31" s="43">
+        <v>5.9391037362319556</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="40">
+        <v>45474</v>
+      </c>
+      <c r="B32" s="41">
+        <v>668</v>
+      </c>
+      <c r="C32" s="41">
+        <v>994.68</v>
+      </c>
+      <c r="D32" s="41">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>716.096</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>38.1197408297894</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>0.67797625917021065</v>
+      </c>
+      <c r="H32" s="53">
+        <f t="shared" si="4"/>
+        <v>94.67672758543695</v>
+      </c>
+      <c r="I32" s="30">
+        <f t="shared" si="2"/>
+        <v>267.2</v>
+      </c>
+      <c r="J32" s="48">
+        <f t="shared" si="5"/>
+        <v>1585.9033876765286</v>
+      </c>
+      <c r="K32" s="48">
+        <f t="shared" si="6"/>
+        <v>558.06919272000005</v>
+      </c>
+      <c r="L32" s="48">
+        <f t="shared" si="7"/>
+        <v>1027.8341949565286</v>
+      </c>
+      <c r="M32" s="23">
+        <v>0.56105400000000005</v>
+      </c>
+      <c r="N32">
+        <v>2.68</v>
+      </c>
+      <c r="O32" s="28">
+        <v>5.7065480284115871E-2</v>
+      </c>
+      <c r="P32" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q32" s="43">
+        <v>5.9352671694480863</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="40">
+        <v>45505</v>
+      </c>
+      <c r="B33" s="41">
+        <v>0</v>
+      </c>
+      <c r="C33" s="41">
+        <v>0</v>
+      </c>
+      <c r="D33" s="41">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="23">
+        <v>0.52071100000000003</v>
+      </c>
+      <c r="N33">
+        <v>2.68</v>
+      </c>
+      <c r="O33" s="28">
+        <v>7.3904145474031777E-2</v>
+      </c>
+      <c r="P33" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q33" s="43">
+        <v>5.9554631704407912</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="40">
+        <v>45536</v>
+      </c>
+      <c r="B34" s="41">
+        <v>0</v>
+      </c>
+      <c r="C34" s="41">
+        <v>0</v>
+      </c>
+      <c r="D34" s="41">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="23">
+        <v>0.50722400000000001</v>
+      </c>
+      <c r="N34">
+        <v>2.68</v>
+      </c>
+      <c r="O34" s="28">
+        <v>9.1656076504074896E-2</v>
+      </c>
+      <c r="P34" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q34" s="43">
+        <v>5.9398075895241602</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="40">
+        <v>45566</v>
+      </c>
+      <c r="B35" s="41">
+        <v>104</v>
+      </c>
+      <c r="C35" s="41">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="D35" s="41">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>111.48800000000001</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>11.723674217312112</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>9.9764325782687902E-2</v>
+      </c>
+      <c r="H35" s="53">
+        <f t="shared" si="4"/>
+        <v>89.48436224767498</v>
+      </c>
+      <c r="I35" s="30">
+        <f t="shared" si="2"/>
+        <v>41.6</v>
+      </c>
+      <c r="J35" s="48">
+        <f t="shared" si="5"/>
+        <v>251.23115011307976</v>
+      </c>
+      <c r="K35" s="48">
+        <f t="shared" si="6"/>
+        <v>75.466517400000015</v>
+      </c>
+      <c r="L35" s="48">
+        <f t="shared" si="7"/>
+        <v>175.76463271307975</v>
+      </c>
+      <c r="M35" s="19">
+        <v>0.51760300000000004</v>
+      </c>
+      <c r="N35">
+        <v>2.68</v>
+      </c>
+      <c r="O35" s="28">
+        <v>0.11272763670492415</v>
+      </c>
+      <c r="P35" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q35" s="43">
+        <v>6.0392103392567247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="40">
+        <v>45597</v>
+      </c>
+      <c r="B36" s="41">
+        <v>194</v>
+      </c>
+      <c r="C36" s="41">
+        <v>324</v>
+      </c>
+      <c r="D36" s="41">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>207.96799999999999</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>13.595054671944959</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>0.19437294532805505</v>
+      </c>
+      <c r="H36" s="53">
+        <f t="shared" si="4"/>
+        <v>93.462910316998318</v>
+      </c>
+      <c r="I36" s="30">
+        <f t="shared" si="2"/>
+        <v>77.599999999999994</v>
+      </c>
+      <c r="J36" s="48">
+        <f t="shared" si="5"/>
+        <v>468.6427223263218</v>
+      </c>
+      <c r="K36" s="48">
+        <f t="shared" si="6"/>
+        <v>167.49665999999999</v>
+      </c>
+      <c r="L36" s="48">
+        <f t="shared" si="7"/>
+        <v>301.14606232632184</v>
+      </c>
+      <c r="M36" s="19">
+        <v>0.51696500000000001</v>
+      </c>
+      <c r="N36">
+        <v>2.68</v>
+      </c>
+      <c r="O36" s="28">
+        <v>7.0077601401778142E-2</v>
+      </c>
+      <c r="P36" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q36" s="43">
+        <v>6.0392103392567247</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="40">
+        <v>45627</v>
+      </c>
+      <c r="B37" s="41">
+        <v>74</v>
+      </c>
+      <c r="C37" s="41">
+        <v>93.96</v>
+      </c>
+      <c r="D37" s="41">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>79.328000000000003</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>4.1711398229826031</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>7.5156860177017393E-2</v>
+      </c>
+      <c r="H37" s="53">
+        <f t="shared" si="4"/>
+        <v>94.741907242105427</v>
+      </c>
+      <c r="I37" s="30">
+        <f t="shared" si="2"/>
+        <v>29.6</v>
+      </c>
+      <c r="J37" s="48">
+        <f t="shared" si="5"/>
+        <v>178.76062604199905</v>
+      </c>
+      <c r="K37" s="48">
+        <f t="shared" si="6"/>
+        <v>48.859575839999998</v>
+      </c>
+      <c r="L37" s="48">
+        <f t="shared" si="7"/>
+        <v>129.90105020199906</v>
+      </c>
+      <c r="M37" s="19">
+        <v>0.52000400000000002</v>
+      </c>
+      <c r="N37">
+        <v>2.68</v>
+      </c>
+      <c r="O37" s="28">
+        <v>5.6366754364629776E-2</v>
+      </c>
+      <c r="P37" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q37" s="43">
+        <v>6.0392103392567247</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="37"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B40" s="38"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649C53B8-6E9B-438C-A5DA-F2FD7BD79411}">
+  <dimension ref="A1:Q41"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="40">
+        <v>44562</v>
+      </c>
+      <c r="B2" s="32">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32">
+        <v>0</v>
+      </c>
+      <c r="D2" s="32">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E37" si="0">(B2/P2)*N2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F37" si="1">B2*O2</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>(E2-F2)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="47" t="e">
+        <f t="shared" ref="H2:H37" si="2">(E2-F2)/E2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I2" s="30">
+        <f t="shared" ref="I2:I37" si="3">B2/P2</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="48">
+        <f>I2*Q2</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="48">
+        <f>C2*M2</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="48">
+        <f>J2-K2</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="21">
+        <v>0.40167399999999998</v>
+      </c>
+      <c r="N2">
+        <v>2.68</v>
+      </c>
+      <c r="O2" s="28">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="P2" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q2" s="43">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="40">
+        <v>44593</v>
+      </c>
+      <c r="B3" s="32">
+        <v>0</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0</v>
+      </c>
+      <c r="D3" s="32">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G37" si="4">(E3-F3)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="47" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I3" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="48">
+        <f t="shared" ref="J3:J37" si="5">I3*Q3</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="48">
+        <f t="shared" ref="K3:K37" si="6">C3*M3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="48">
+        <f t="shared" ref="L3:L37" si="7">J3-K3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="21">
+        <v>0.41300100000000001</v>
+      </c>
+      <c r="N3">
+        <v>2.68</v>
+      </c>
+      <c r="O3" s="28">
+        <v>5.0254040888372771E-2</v>
+      </c>
+      <c r="P3" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q3" s="43">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="40">
+        <v>44621</v>
+      </c>
+      <c r="B4" s="32">
+        <v>250.22</v>
+      </c>
+      <c r="C4" s="32">
+        <v>440.64</v>
+      </c>
+      <c r="D4" s="49">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>268.23584</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>10.162721642192826</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="4"/>
+        <v>0.25807311835780716</v>
+      </c>
+      <c r="H4" s="52">
+        <f>((E4-F4)/E4)*100</f>
+        <v>96.211273764835894</v>
+      </c>
+      <c r="I4" s="30">
+        <f t="shared" si="3"/>
+        <v>100.08799999999999</v>
+      </c>
+      <c r="J4" s="48">
+        <f t="shared" si="5"/>
+        <v>627.55175999999994</v>
+      </c>
+      <c r="K4" s="48">
+        <f t="shared" si="6"/>
+        <v>176.6591856</v>
+      </c>
+      <c r="L4" s="48">
+        <f t="shared" si="7"/>
+        <v>450.89257439999994</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0.40091500000000002</v>
+      </c>
+      <c r="N4">
+        <v>2.68</v>
+      </c>
+      <c r="O4" s="28">
+        <v>4.0615145240959265E-2</v>
+      </c>
+      <c r="P4" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q4" s="43">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="40">
+        <v>44652</v>
+      </c>
+      <c r="B5" s="32">
+        <v>648.45000000000005</v>
+      </c>
+      <c r="C5" s="32">
+        <v>1172.8800000000001</v>
+      </c>
+      <c r="D5" s="49">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>695.13840000000005</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>13.9988327130439</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>0.68113956728695613</v>
+      </c>
+      <c r="H5" s="52">
+        <f t="shared" ref="H5:H37" si="8">((E5-F5)/E5)*100</f>
+        <v>97.986180491101635</v>
+      </c>
+      <c r="I5" s="30">
+        <f t="shared" si="3"/>
+        <v>259.38</v>
+      </c>
+      <c r="J5" s="48">
+        <f t="shared" si="5"/>
+        <v>1714.5018</v>
+      </c>
+      <c r="K5" s="48">
+        <f t="shared" si="6"/>
+        <v>479.06987328000002</v>
+      </c>
+      <c r="L5" s="48">
+        <f t="shared" si="7"/>
+        <v>1235.4319267199999</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0.40845599999999999</v>
+      </c>
+      <c r="N5">
+        <v>2.68</v>
+      </c>
+      <c r="O5" s="28">
+        <v>2.1588145135390389E-2</v>
+      </c>
+      <c r="P5" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q5" s="43">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="40">
+        <v>44682</v>
+      </c>
+      <c r="B6" s="32">
+        <v>2040</v>
+      </c>
+      <c r="C6" s="32">
+        <v>3204.36</v>
+      </c>
+      <c r="D6" s="49">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2186.88</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>57.171464867888183</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>2.1297085351321119</v>
+      </c>
+      <c r="H6" s="52">
+        <f t="shared" si="8"/>
+        <v>97.385706354811958</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" si="3"/>
+        <v>816</v>
+      </c>
+      <c r="J6" s="48">
+        <f t="shared" si="5"/>
+        <v>5597.76</v>
+      </c>
+      <c r="K6" s="48">
+        <f t="shared" si="6"/>
+        <v>1328.14633716</v>
+      </c>
+      <c r="L6" s="48">
+        <f t="shared" si="7"/>
+        <v>4269.61366284</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0.41448099999999999</v>
+      </c>
+      <c r="N6">
+        <v>2.68</v>
+      </c>
+      <c r="O6" s="28">
+        <v>2.8025227876415777E-2</v>
+      </c>
+      <c r="P6" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q6" s="43">
+        <v>6.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="40">
+        <v>44713</v>
+      </c>
+      <c r="B7" s="32">
+        <v>539.5</v>
+      </c>
+      <c r="C7" s="32">
+        <v>849</v>
+      </c>
+      <c r="D7" s="49">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>578.34400000000005</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>23.77069640308547</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>0.55457330359691459</v>
+      </c>
+      <c r="H7" s="52">
+        <f t="shared" si="8"/>
+        <v>95.889868935601399</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" si="3"/>
+        <v>215.8</v>
+      </c>
+      <c r="J7" s="48">
+        <f t="shared" si="5"/>
+        <v>1553.7600000000002</v>
+      </c>
+      <c r="K7" s="48">
+        <f t="shared" si="6"/>
+        <v>347.74530600000003</v>
+      </c>
+      <c r="L7" s="48">
+        <f t="shared" si="7"/>
+        <v>1206.0146940000002</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0.40959400000000001</v>
+      </c>
+      <c r="N7">
+        <v>2.68</v>
+      </c>
+      <c r="O7" s="28">
+        <v>4.4060605010353047E-2</v>
+      </c>
+      <c r="P7" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q7" s="43">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
+        <v>44743</v>
+      </c>
+      <c r="B8" s="32">
+        <v>2494.5700000000002</v>
+      </c>
+      <c r="C8" s="32">
+        <v>3622.32</v>
+      </c>
+      <c r="D8" s="49">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2674.1790400000004</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>104.43698760989382</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>2.5697420523901062</v>
+      </c>
+      <c r="H8" s="52">
+        <f t="shared" si="8"/>
+        <v>96.094614980981447</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="shared" si="3"/>
+        <v>997.82800000000009</v>
+      </c>
+      <c r="J8" s="48">
+        <f t="shared" si="5"/>
+        <v>7413.86204</v>
+      </c>
+      <c r="K8" s="48">
+        <f t="shared" si="6"/>
+        <v>1361.7025343999999</v>
+      </c>
+      <c r="L8" s="48">
+        <f t="shared" si="7"/>
+        <v>6052.1595056000006</v>
+      </c>
+      <c r="M8" s="21">
+        <v>0.37591999999999998</v>
+      </c>
+      <c r="N8">
+        <v>2.68</v>
+      </c>
+      <c r="O8" s="28">
+        <v>4.1865727403878748E-2</v>
+      </c>
+      <c r="P8" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q8" s="43">
+        <v>7.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>44774</v>
+      </c>
+      <c r="B9" s="32">
+        <v>3246.84</v>
+      </c>
+      <c r="C9" s="32">
+        <v>4390.2</v>
+      </c>
+      <c r="D9" s="49">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3480.6124800000007</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>148.42629658584264</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>3.3321861834141582</v>
+      </c>
+      <c r="H9" s="52">
+        <f t="shared" si="8"/>
+        <v>95.735627064526227</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="3"/>
+        <v>1298.7360000000001</v>
+      </c>
+      <c r="J9" s="48">
+        <f t="shared" si="5"/>
+        <v>9208.0382399999999</v>
+      </c>
+      <c r="K9" s="48">
+        <f t="shared" si="6"/>
+        <v>1812.0594401999999</v>
+      </c>
+      <c r="L9" s="48">
+        <f t="shared" si="7"/>
+        <v>7395.9787998000002</v>
+      </c>
+      <c r="M9" s="21">
+        <v>0.41275099999999998</v>
+      </c>
+      <c r="N9">
+        <v>2.68</v>
+      </c>
+      <c r="O9" s="28">
+        <v>4.5714077868278892E-2</v>
+      </c>
+      <c r="P9" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q9" s="43">
+        <v>7.09</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="40">
+        <v>44805</v>
+      </c>
+      <c r="B10" s="32">
+        <v>0</v>
+      </c>
+      <c r="C10" s="32">
+        <v>0</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="52" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="21">
+        <v>0.415877</v>
+      </c>
+      <c r="N10">
+        <v>2.68</v>
+      </c>
+      <c r="O10" s="28">
+        <v>4.9086599685372614E-2</v>
+      </c>
+      <c r="P10" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q10" s="43">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
+        <v>44835</v>
+      </c>
+      <c r="B11" s="32">
+        <v>2185.48</v>
+      </c>
+      <c r="C11" s="32">
+        <v>3285.36</v>
+      </c>
+      <c r="D11" s="49">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2342.8345600000002</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>102.9910079780575</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>2.2398435520219429</v>
+      </c>
+      <c r="H11" s="52">
+        <f t="shared" si="8"/>
+        <v>95.603999969248463</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" si="3"/>
+        <v>874.19200000000001</v>
+      </c>
+      <c r="J11" s="48">
+        <f t="shared" si="5"/>
+        <v>5656.0222400000002</v>
+      </c>
+      <c r="K11" s="48">
+        <f t="shared" si="6"/>
+        <v>1358.8051838400002</v>
+      </c>
+      <c r="L11" s="48">
+        <f t="shared" si="7"/>
+        <v>4297.2170561599996</v>
+      </c>
+      <c r="M11" s="21">
+        <v>0.41359400000000002</v>
+      </c>
+      <c r="N11">
+        <v>2.68</v>
+      </c>
+      <c r="O11" s="28">
+        <v>4.7125120329656413E-2</v>
+      </c>
+      <c r="P11" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q11" s="43">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="40">
+        <v>44866</v>
+      </c>
+      <c r="B12" s="32">
+        <v>2517.87</v>
+      </c>
+      <c r="C12" s="32">
+        <v>4205.5200000000004</v>
+      </c>
+      <c r="D12" s="49">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2699.1566399999997</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>101.32767145924649</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>2.5978289685407532</v>
+      </c>
+      <c r="H12" s="52">
+        <f t="shared" si="8"/>
+        <v>96.245950681126573</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="3"/>
+        <v>1007.1479999999999</v>
+      </c>
+      <c r="J12" s="48">
+        <f t="shared" si="5"/>
+        <v>6546.4619999999995</v>
+      </c>
+      <c r="K12" s="48">
+        <f t="shared" si="6"/>
+        <v>1728.98179344</v>
+      </c>
+      <c r="L12" s="48">
+        <f t="shared" si="7"/>
+        <v>4817.4802065599997</v>
+      </c>
+      <c r="M12" s="21">
+        <v>0.41112199999999999</v>
+      </c>
+      <c r="N12">
+        <v>2.68</v>
+      </c>
+      <c r="O12" s="28">
+        <v>4.0243408698322984E-2</v>
+      </c>
+      <c r="P12" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q12" s="43">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="40">
+        <v>44896</v>
+      </c>
+      <c r="B13" s="32">
+        <v>712.76</v>
+      </c>
+      <c r="C13" s="32">
+        <v>1166.4000000000001</v>
+      </c>
+      <c r="D13" s="49">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>764.07871999999998</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>20.93268083994775</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>0.74314603916005217</v>
+      </c>
+      <c r="H13" s="52">
+        <f t="shared" si="8"/>
+        <v>97.260402587844894</v>
+      </c>
+      <c r="I13" s="30">
+        <f t="shared" si="3"/>
+        <v>285.10399999999998</v>
+      </c>
+      <c r="J13" s="48">
+        <f t="shared" si="5"/>
+        <v>1810.4103999999998</v>
+      </c>
+      <c r="K13" s="48">
+        <f t="shared" si="6"/>
+        <v>487.1049696</v>
+      </c>
+      <c r="L13" s="48">
+        <f t="shared" si="7"/>
+        <v>1323.3054303999998</v>
+      </c>
+      <c r="M13" s="21">
+        <v>0.41761399999999999</v>
+      </c>
+      <c r="N13">
+        <v>2.68</v>
+      </c>
+      <c r="O13" s="28">
+        <v>2.9368484258302584E-2</v>
+      </c>
+      <c r="P13" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q13" s="43">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="40">
+        <v>44927</v>
+      </c>
+      <c r="B14" s="32">
+        <v>0</v>
+      </c>
+      <c r="C14" s="32">
+        <v>0</v>
+      </c>
+      <c r="D14" s="32">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="52" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="22">
+        <v>0.41628599999999999</v>
+      </c>
+      <c r="N14">
+        <v>2.68</v>
+      </c>
+      <c r="O14" s="28">
+        <v>2.9173607327091757E-2</v>
+      </c>
+      <c r="P14" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q14" s="43">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="40">
+        <v>44958</v>
+      </c>
+      <c r="B15" s="32">
+        <v>35.125000000000298</v>
+      </c>
+      <c r="C15" s="32">
+        <v>48.6</v>
+      </c>
+      <c r="D15" s="32">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>37.654000000000323</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.83505382362527236</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>3.6818946176375052E-2</v>
+      </c>
+      <c r="H15" s="52">
+        <f t="shared" si="8"/>
+        <v>97.782297169954674</v>
+      </c>
+      <c r="I15" s="30">
+        <f t="shared" si="3"/>
+        <v>14.05000000000012</v>
+      </c>
+      <c r="J15" s="48">
+        <f t="shared" si="5"/>
+        <v>85.143000000000725</v>
+      </c>
+      <c r="K15" s="48">
+        <f t="shared" si="6"/>
+        <v>20.671426799999999</v>
+      </c>
+      <c r="L15" s="48">
+        <f t="shared" si="7"/>
+        <v>64.471573200000734</v>
+      </c>
+      <c r="M15" s="22">
+        <v>0.42533799999999999</v>
+      </c>
+      <c r="N15">
+        <v>2.68</v>
+      </c>
+      <c r="O15" s="28">
+        <v>2.3773774338085845E-2</v>
+      </c>
+      <c r="P15" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q15" s="43">
+        <v>6.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="40">
+        <v>44986</v>
+      </c>
+      <c r="B16" s="32">
+        <v>29.975000000001998</v>
+      </c>
+      <c r="C16" s="32">
+        <v>45.36</v>
+      </c>
+      <c r="D16" s="32">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>32.133200000002148</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.88644985155586586</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>3.124675014844628E-2</v>
+      </c>
+      <c r="H16" s="52">
+        <f t="shared" si="8"/>
+        <v>97.24132718946197</v>
+      </c>
+      <c r="I16" s="30">
+        <f t="shared" si="3"/>
+        <v>11.9900000000008</v>
+      </c>
+      <c r="J16" s="48">
+        <f t="shared" si="5"/>
+        <v>70.3813000000047</v>
+      </c>
+      <c r="K16" s="48">
+        <f t="shared" si="6"/>
+        <v>19.397795760000001</v>
+      </c>
+      <c r="L16" s="48">
+        <f t="shared" si="7"/>
+        <v>50.983504240004699</v>
+      </c>
+      <c r="M16" s="22">
+        <v>0.42764099999999999</v>
+      </c>
+      <c r="N16">
+        <v>2.68</v>
+      </c>
+      <c r="O16" s="28">
+        <v>2.9572972528967699E-2</v>
+      </c>
+      <c r="P16" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q16" s="43">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="40">
+        <v>45017</v>
+      </c>
+      <c r="B17" s="32">
+        <v>22.629999999996997</v>
+      </c>
+      <c r="C17" s="32">
+        <v>68.040000000000006</v>
+      </c>
+      <c r="D17" s="32">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>24.259359999996782</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.77002543539074098</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>2.348933456460604E-2</v>
+      </c>
+      <c r="H17" s="52">
+        <f t="shared" si="8"/>
+        <v>96.825862531448294</v>
+      </c>
+      <c r="I17" s="30">
+        <f t="shared" si="3"/>
+        <v>9.0519999999987988</v>
+      </c>
+      <c r="J17" s="48">
+        <f t="shared" si="5"/>
+        <v>51.958479999993109</v>
+      </c>
+      <c r="K17" s="48">
+        <f t="shared" si="6"/>
+        <v>28.423778040000002</v>
+      </c>
+      <c r="L17" s="48">
+        <f t="shared" si="7"/>
+        <v>23.534701959993107</v>
+      </c>
+      <c r="M17" s="22">
+        <v>0.41775099999999998</v>
+      </c>
+      <c r="N17">
+        <v>2.68</v>
+      </c>
+      <c r="O17" s="28">
+        <v>3.40267536628742E-2</v>
+      </c>
+      <c r="P17" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q17" s="43">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="40">
+        <v>45047</v>
+      </c>
+      <c r="B18" s="32">
+        <v>109.48000000000302</v>
+      </c>
+      <c r="C18" s="32">
+        <v>171.72</v>
+      </c>
+      <c r="D18" s="32">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>117.36256000000324</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>3.2308405317611215</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>0.11413171946824212</v>
+      </c>
+      <c r="H18" s="52">
+        <f t="shared" si="8"/>
+        <v>97.247128443891285</v>
+      </c>
+      <c r="I18" s="30">
+        <f t="shared" si="3"/>
+        <v>43.79200000000121</v>
+      </c>
+      <c r="J18" s="48">
+        <f t="shared" si="5"/>
+        <v>235.60096000000649</v>
+      </c>
+      <c r="K18" s="48">
+        <f t="shared" si="6"/>
+        <v>72.225775439999992</v>
+      </c>
+      <c r="L18" s="48">
+        <f t="shared" si="7"/>
+        <v>163.37518456000652</v>
+      </c>
+      <c r="M18" s="22">
+        <v>0.42060199999999998</v>
+      </c>
+      <c r="N18">
+        <v>2.68</v>
+      </c>
+      <c r="O18" s="28">
+        <v>2.9510783081485501E-2</v>
+      </c>
+      <c r="P18" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q18" s="43">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="40">
+        <v>45078</v>
+      </c>
+      <c r="B19" s="32">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="C19" s="32">
+        <v>51.84</v>
+      </c>
+      <c r="D19" s="32">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>37.4664</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>1.844933734890428</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>3.5621466265109578E-2</v>
+      </c>
+      <c r="H19" s="52">
+        <f t="shared" si="8"/>
+        <v>95.075764592033323</v>
+      </c>
+      <c r="I19" s="30">
+        <f t="shared" si="3"/>
+        <v>13.98</v>
+      </c>
+      <c r="J19" s="48">
+        <f t="shared" si="5"/>
+        <v>70.599000000000004</v>
+      </c>
+      <c r="K19" s="48">
+        <f t="shared" si="6"/>
+        <v>22.13469504</v>
+      </c>
+      <c r="L19" s="48">
+        <f t="shared" si="7"/>
+        <v>48.464304960000007</v>
+      </c>
+      <c r="M19" s="22">
+        <v>0.426981</v>
+      </c>
+      <c r="N19">
+        <v>2.68</v>
+      </c>
+      <c r="O19" s="28">
+        <v>5.2787803573402799E-2</v>
+      </c>
+      <c r="P19" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q19" s="43">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="40">
+        <v>45108</v>
+      </c>
+      <c r="B20" s="32">
+        <v>27.810000000001004</v>
+      </c>
+      <c r="C20" s="32">
+        <v>42.12</v>
+      </c>
+      <c r="D20" s="32">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>29.81232000000108</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>1.3768733826192685</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>2.8435446617381812E-2</v>
+      </c>
+      <c r="H20" s="52">
+        <f t="shared" si="8"/>
+        <v>95.38152890275154</v>
+      </c>
+      <c r="I20" s="30">
+        <f t="shared" si="3"/>
+        <v>11.124000000000402</v>
+      </c>
+      <c r="J20" s="48">
+        <f t="shared" si="5"/>
+        <v>55.620000000002008</v>
+      </c>
+      <c r="K20" s="48">
+        <f t="shared" si="6"/>
+        <v>18.29490624</v>
+      </c>
+      <c r="L20" s="48">
+        <f t="shared" si="7"/>
+        <v>37.325093760002005</v>
+      </c>
+      <c r="M20" s="22">
+        <v>0.43435200000000002</v>
+      </c>
+      <c r="N20">
+        <v>2.68</v>
+      </c>
+      <c r="O20" s="28">
+        <v>4.9510010162503372E-2</v>
+      </c>
+      <c r="P20" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q20" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="40">
+        <v>45139</v>
+      </c>
+      <c r="B21" s="32">
+        <v>507</v>
+      </c>
+      <c r="C21" s="32">
+        <v>793.8</v>
+      </c>
+      <c r="D21" s="32">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>543.50400000000002</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>21.243739609343965</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>0.52226026039065609</v>
+      </c>
+      <c r="H21" s="52">
+        <f t="shared" si="8"/>
+        <v>96.091337026159152</v>
+      </c>
+      <c r="I21" s="30">
+        <f t="shared" si="3"/>
+        <v>202.8</v>
+      </c>
+      <c r="J21" s="48">
+        <f t="shared" si="5"/>
+        <v>1121.4840000000002</v>
+      </c>
+      <c r="K21" s="48">
+        <f t="shared" si="6"/>
+        <v>391.77205199999997</v>
+      </c>
+      <c r="L21" s="48">
+        <f t="shared" si="7"/>
+        <v>729.71194800000012</v>
+      </c>
+      <c r="M21" s="22">
+        <v>0.49353999999999998</v>
+      </c>
+      <c r="N21">
+        <v>2.68</v>
+      </c>
+      <c r="O21" s="28">
+        <v>4.1900867079573897E-2</v>
+      </c>
+      <c r="P21" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q21" s="43">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="40">
+        <v>45170</v>
+      </c>
+      <c r="B22" s="32">
+        <v>607</v>
+      </c>
+      <c r="C22" s="32">
+        <v>1078.92</v>
+      </c>
+      <c r="D22" s="32">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>650.70400000000006</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>20.841026867019099</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>0.62986297313298101</v>
+      </c>
+      <c r="H22" s="52">
+        <f t="shared" si="8"/>
+        <v>96.797157099538495</v>
+      </c>
+      <c r="I22" s="30">
+        <f t="shared" si="3"/>
+        <v>242.8</v>
+      </c>
+      <c r="J22" s="48">
+        <f t="shared" si="5"/>
+        <v>1473.796</v>
+      </c>
+      <c r="K22" s="48">
+        <f t="shared" si="6"/>
+        <v>599.00235803999999</v>
+      </c>
+      <c r="L22" s="48">
+        <f t="shared" si="7"/>
+        <v>874.79364196000006</v>
+      </c>
+      <c r="M22" s="22">
+        <v>0.55518699999999999</v>
+      </c>
+      <c r="N22">
+        <v>2.68</v>
+      </c>
+      <c r="O22" s="28">
+        <v>3.4334475892947448E-2</v>
+      </c>
+      <c r="P22" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q22" s="43">
+        <v>6.07</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="40">
+        <v>45200</v>
+      </c>
+      <c r="B23" s="32">
+        <v>1650.7100000000028</v>
+      </c>
+      <c r="C23" s="32">
+        <v>3330.72</v>
+      </c>
+      <c r="D23" s="32">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>1769.561120000003</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>63.931335935890601</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>1.7056297840641126</v>
+      </c>
+      <c r="H23" s="52">
+        <f t="shared" si="8"/>
+        <v>96.387164296653935</v>
+      </c>
+      <c r="I23" s="30">
+        <f t="shared" si="3"/>
+        <v>660.28400000000113</v>
+      </c>
+      <c r="J23" s="48">
+        <f t="shared" si="5"/>
+        <v>4014.5267200000071</v>
+      </c>
+      <c r="K23" s="48">
+        <f t="shared" si="6"/>
+        <v>1797.1066295999999</v>
+      </c>
+      <c r="L23" s="48">
+        <f t="shared" si="7"/>
+        <v>2217.4200904000072</v>
+      </c>
+      <c r="M23" s="22">
+        <v>0.53955500000000001</v>
+      </c>
+      <c r="N23">
+        <v>2.68</v>
+      </c>
+      <c r="O23" s="28">
+        <v>3.8729598739869808E-2</v>
+      </c>
+      <c r="P23" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q23" s="43">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="40">
+        <v>45231</v>
+      </c>
+      <c r="B24" s="32">
+        <v>2305</v>
+      </c>
+      <c r="C24" s="32">
+        <v>3525.12</v>
+      </c>
+      <c r="D24" s="32">
+        <v>17</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>2470.96</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>121.99367485137363</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>2.3489663251486261</v>
+      </c>
+      <c r="H24" s="52">
+        <f t="shared" si="8"/>
+        <v>95.062903695269299</v>
+      </c>
+      <c r="I24" s="30">
+        <f t="shared" si="3"/>
+        <v>922</v>
+      </c>
+      <c r="J24" s="48">
+        <f t="shared" si="5"/>
+        <v>5605.76</v>
+      </c>
+      <c r="K24" s="48">
+        <f t="shared" si="6"/>
+        <v>1904.8585190400001</v>
+      </c>
+      <c r="L24" s="48">
+        <f t="shared" si="7"/>
+        <v>3700.9014809600003</v>
+      </c>
+      <c r="M24" s="22">
+        <v>0.54036700000000004</v>
+      </c>
+      <c r="N24">
+        <v>2.68</v>
+      </c>
+      <c r="O24" s="28">
+        <v>5.2925672386713071E-2</v>
+      </c>
+      <c r="P24" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q24" s="43">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="40">
+        <v>45261</v>
+      </c>
+      <c r="B25" s="32">
+        <v>551</v>
+      </c>
+      <c r="C25" s="29">
+        <v>855.36</v>
+      </c>
+      <c r="D25" s="32">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>590.67200000000003</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>25.273520656496345</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>0.56539847934350373</v>
+      </c>
+      <c r="H25" s="52">
+        <f t="shared" si="8"/>
+        <v>95.721225882300786</v>
+      </c>
+      <c r="I25" s="30">
+        <f t="shared" si="3"/>
+        <v>220.4</v>
+      </c>
+      <c r="J25" s="48">
+        <f t="shared" si="5"/>
+        <v>1309.1760000000002</v>
+      </c>
+      <c r="K25" s="48">
+        <f t="shared" si="6"/>
+        <v>464.82144191999998</v>
+      </c>
+      <c r="L25" s="48">
+        <f t="shared" si="7"/>
+        <v>844.35455808000017</v>
+      </c>
+      <c r="M25" s="23">
+        <v>0.54342199999999996</v>
+      </c>
+      <c r="N25">
+        <v>2.68</v>
+      </c>
+      <c r="O25" s="28">
+        <v>4.586845854173565E-2</v>
+      </c>
+      <c r="P25" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q25" s="43">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="40">
+        <v>45292</v>
+      </c>
+      <c r="B26" s="33">
+        <v>2819</v>
+      </c>
+      <c r="C26" s="35">
+        <v>3291.8399999999997</v>
+      </c>
+      <c r="D26" s="33">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>3021.9679999999998</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>118.68031396742798</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>2.9032876860325718</v>
+      </c>
+      <c r="H26" s="52">
+        <f t="shared" si="8"/>
+        <v>96.072747495425887</v>
+      </c>
+      <c r="I26" s="30">
+        <f t="shared" si="3"/>
+        <v>1127.5999999999999</v>
+      </c>
+      <c r="J26" s="48">
+        <f t="shared" si="5"/>
+        <v>6630.2879999999996</v>
+      </c>
+      <c r="K26" s="48">
+        <f t="shared" si="6"/>
+        <v>1803.3226214399997</v>
+      </c>
+      <c r="L26" s="48">
+        <f t="shared" si="7"/>
+        <v>4826.9653785600003</v>
+      </c>
+      <c r="M26" s="22">
+        <v>0.54781599999999997</v>
+      </c>
+      <c r="N26">
+        <v>2.68</v>
+      </c>
+      <c r="O26" s="28">
+        <v>4.2100146849034403E-2</v>
+      </c>
+      <c r="P26" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q26" s="43">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="40">
+        <v>45323</v>
+      </c>
+      <c r="B27" s="34">
+        <v>2748</v>
+      </c>
+      <c r="C27" s="50">
+        <v>2841.4800000000005</v>
+      </c>
+      <c r="D27" s="34">
+        <v>14</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>2945.8560000000002</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>103.25926592061819</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>2.8425967340793821</v>
+      </c>
+      <c r="H27" s="52">
+        <f t="shared" si="8"/>
+        <v>96.49476193267364</v>
+      </c>
+      <c r="I27" s="30">
+        <f t="shared" si="3"/>
+        <v>1099.2</v>
+      </c>
+      <c r="J27" s="48">
+        <f t="shared" si="5"/>
+        <v>6463.2960000000003</v>
+      </c>
+      <c r="K27" s="48">
+        <f t="shared" si="6"/>
+        <v>1565.0502447600004</v>
+      </c>
+      <c r="L27" s="48">
+        <f t="shared" si="7"/>
+        <v>4898.2457552400001</v>
+      </c>
+      <c r="M27" s="22">
+        <v>0.55078700000000003</v>
+      </c>
+      <c r="N27">
+        <v>2.68</v>
+      </c>
+      <c r="O27" s="28">
+        <v>3.7576152081738791E-2</v>
+      </c>
+      <c r="P27" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q27" s="43">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="40">
+        <v>45352</v>
+      </c>
+      <c r="B28" s="35">
+        <v>1056</v>
+      </c>
+      <c r="C28" s="35">
+        <v>1202.04</v>
+      </c>
+      <c r="D28" s="35">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1132.0319999999999</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>29.34727056101924</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>1.1026847294389805</v>
+      </c>
+      <c r="H28" s="52">
+        <f t="shared" si="8"/>
+        <v>97.40755821734551</v>
+      </c>
+      <c r="I28" s="30">
+        <f t="shared" si="3"/>
+        <v>422.4</v>
+      </c>
+      <c r="J28" s="48">
+        <f t="shared" si="5"/>
+        <v>2193.6512407619584</v>
+      </c>
+      <c r="K28" s="48">
+        <f t="shared" si="6"/>
+        <v>657.50506164000001</v>
+      </c>
+      <c r="L28" s="48">
+        <f t="shared" si="7"/>
+        <v>1536.1461791219585</v>
+      </c>
+      <c r="M28" s="23">
+        <v>0.546991</v>
+      </c>
+      <c r="N28">
+        <v>2.68</v>
+      </c>
+      <c r="O28" s="28">
+        <v>2.7790975910056099E-2</v>
+      </c>
+      <c r="P28" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q28" s="43">
+        <v>5.1933031268038796</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="40">
+        <v>45383</v>
+      </c>
+      <c r="B29" s="35">
+        <v>885</v>
+      </c>
+      <c r="C29" s="35">
+        <v>1140.48</v>
+      </c>
+      <c r="D29" s="35">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>948.72</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>17.225145882981881</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>0.93149485411701816</v>
+      </c>
+      <c r="H29" s="52">
+        <f t="shared" si="8"/>
+        <v>98.184380440700963</v>
+      </c>
+      <c r="I29" s="30">
+        <f t="shared" si="3"/>
+        <v>354</v>
+      </c>
+      <c r="J29" s="48">
+        <f t="shared" si="5"/>
+        <v>2087.7503999999999</v>
+      </c>
+      <c r="K29" s="48">
+        <f t="shared" si="6"/>
+        <v>615.31861247999996</v>
+      </c>
+      <c r="L29" s="48">
+        <f t="shared" si="7"/>
+        <v>1472.4317875199999</v>
+      </c>
+      <c r="M29" s="23">
+        <v>0.53952599999999995</v>
+      </c>
+      <c r="N29">
+        <v>2.68</v>
+      </c>
+      <c r="O29" s="28">
+        <v>1.9463441675685741E-2</v>
+      </c>
+      <c r="P29" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q29" s="43">
+        <v>5.8975999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="40">
+        <v>45413</v>
+      </c>
+      <c r="B30" s="35">
+        <v>1006</v>
+      </c>
+      <c r="C30" s="35">
+        <v>1052.9999999999998</v>
+      </c>
+      <c r="D30" s="35">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1078.432</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>28.512749151828793</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="4"/>
+        <v>1.0499192508481712</v>
+      </c>
+      <c r="H30" s="52">
+        <f t="shared" si="8"/>
+        <v>97.356092071467756</v>
+      </c>
+      <c r="I30" s="30">
+        <f t="shared" si="3"/>
+        <v>402.4</v>
+      </c>
+      <c r="J30" s="48">
+        <f t="shared" si="5"/>
+        <v>2375.9910734256796</v>
+      </c>
+      <c r="K30" s="48">
+        <f t="shared" si="6"/>
+        <v>574.68106799999987</v>
+      </c>
+      <c r="L30" s="48">
+        <f t="shared" si="7"/>
+        <v>1801.3100054256797</v>
+      </c>
+      <c r="M30" s="23">
+        <v>0.54575600000000002</v>
+      </c>
+      <c r="N30">
+        <v>2.68</v>
+      </c>
+      <c r="O30" s="28">
+        <v>2.83426929938656E-2</v>
+      </c>
+      <c r="P30" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q30" s="43">
+        <v>5.9045503812765405</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
+        <v>45444</v>
+      </c>
+      <c r="B31" s="31">
+        <v>0</v>
+      </c>
+      <c r="C31" s="31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="52" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="23">
+        <v>0.556674</v>
+      </c>
+      <c r="N31">
+        <v>2.68</v>
+      </c>
+      <c r="O31" s="28">
+        <v>3.6478268557543055E-2</v>
+      </c>
+      <c r="P31" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q31" s="43">
+        <v>5.9391037362319556</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="40">
+        <v>45474</v>
+      </c>
+      <c r="B32" s="31">
+        <v>2339</v>
+      </c>
+      <c r="C32" s="35">
+        <v>2841.4799999999996</v>
+      </c>
+      <c r="D32" s="35">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>2507.4080000000004</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>133.47615838454703</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="4"/>
+        <v>2.3739318416154531</v>
+      </c>
+      <c r="H32" s="52">
+        <f t="shared" si="8"/>
+        <v>94.67672758543695</v>
+      </c>
+      <c r="I32" s="30">
+        <f t="shared" si="3"/>
+        <v>935.6</v>
+      </c>
+      <c r="J32" s="48">
+        <f t="shared" si="5"/>
+        <v>5553.0359637356296</v>
+      </c>
+      <c r="K32" s="48">
+        <f t="shared" si="6"/>
+        <v>1594.2237199199999</v>
+      </c>
+      <c r="L32" s="48">
+        <f t="shared" si="7"/>
+        <v>3958.8122438156297</v>
+      </c>
+      <c r="M32" s="23">
+        <v>0.56105400000000005</v>
+      </c>
+      <c r="N32">
+        <v>2.68</v>
+      </c>
+      <c r="O32" s="28">
+        <v>5.7065480284115871E-2</v>
+      </c>
+      <c r="P32" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q32" s="43">
+        <v>5.9352671694480863</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="40">
+        <v>45505</v>
+      </c>
+      <c r="B33" s="36">
+        <v>525</v>
+      </c>
+      <c r="C33" s="51">
+        <v>680.4</v>
+      </c>
+      <c r="D33" s="36">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>562.80000000000007</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>38.799676373866681</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="4"/>
+        <v>0.52400032362613347</v>
+      </c>
+      <c r="H33" s="52">
+        <f t="shared" si="8"/>
+        <v>93.105956578914956</v>
+      </c>
+      <c r="I33" s="30">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="J33" s="48">
+        <f t="shared" si="5"/>
+        <v>1250.6472657925663</v>
+      </c>
+      <c r="K33" s="48">
+        <f t="shared" si="6"/>
+        <v>354.29176440000003</v>
+      </c>
+      <c r="L33" s="48">
+        <f t="shared" si="7"/>
+        <v>896.35550139256623</v>
+      </c>
+      <c r="M33" s="23">
+        <v>0.52071100000000003</v>
+      </c>
+      <c r="N33">
+        <v>2.68</v>
+      </c>
+      <c r="O33" s="28">
+        <v>7.3904145474031777E-2</v>
+      </c>
+      <c r="P33" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q33" s="43">
+        <v>5.9554631704407912</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="40">
+        <v>45536</v>
+      </c>
+      <c r="B34" s="36">
+        <v>0</v>
+      </c>
+      <c r="C34" s="36">
+        <v>0</v>
+      </c>
+      <c r="D34" s="36">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="52" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="23">
+        <v>0.50722400000000001</v>
+      </c>
+      <c r="N34">
+        <v>2.68</v>
+      </c>
+      <c r="O34" s="28">
+        <v>9.1656076504074896E-2</v>
+      </c>
+      <c r="P34" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q34" s="43">
+        <v>5.9398075895241602</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="40">
+        <v>45566</v>
+      </c>
+      <c r="B35" s="36">
+        <v>137</v>
+      </c>
+      <c r="C35" s="51">
+        <v>343.44000000000005</v>
+      </c>
+      <c r="D35" s="36">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>146.864</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>15.443686228574609</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="4"/>
+        <v>0.13142031377142538</v>
+      </c>
+      <c r="H35" s="52">
+        <f t="shared" si="8"/>
+        <v>89.48436224767498</v>
+      </c>
+      <c r="I35" s="30">
+        <f t="shared" si="3"/>
+        <v>54.8</v>
+      </c>
+      <c r="J35" s="48">
+        <f t="shared" si="5"/>
+        <v>330.9487265912685</v>
+      </c>
+      <c r="K35" s="48">
+        <f t="shared" si="6"/>
+        <v>177.76557432000004</v>
+      </c>
+      <c r="L35" s="48">
+        <f t="shared" si="7"/>
+        <v>153.18315227126845</v>
+      </c>
+      <c r="M35" s="19">
+        <v>0.51760300000000004</v>
+      </c>
+      <c r="N35">
+        <v>2.68</v>
+      </c>
+      <c r="O35" s="28">
+        <v>0.11272763670492415</v>
+      </c>
+      <c r="P35" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q35" s="43">
+        <v>6.0392103392567247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="40">
+        <v>45597</v>
+      </c>
+      <c r="B36" s="36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="52" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I36" s="30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L36" s="48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="19">
+        <v>0.51696500000000001</v>
+      </c>
+      <c r="N36">
+        <v>2.68</v>
+      </c>
+      <c r="O36" s="28">
+        <v>7.0077601401778142E-2</v>
+      </c>
+      <c r="P36" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q36" s="43">
+        <v>6.0392103392567247</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="40">
+        <v>45627</v>
+      </c>
+      <c r="B37" s="36">
+        <v>41</v>
+      </c>
+      <c r="C37" s="51">
+        <v>100.44</v>
+      </c>
+      <c r="D37" s="36">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>43.951999999999998</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>2.3110369289498207</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="4"/>
+        <v>4.1640963071050183E-2</v>
+      </c>
+      <c r="H37" s="52">
+        <f t="shared" si="8"/>
+        <v>94.741907242105441</v>
+      </c>
+      <c r="I37" s="30">
+        <f t="shared" si="3"/>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J37" s="48">
+        <f t="shared" si="5"/>
+        <v>99.043049563810271</v>
+      </c>
+      <c r="K37" s="48">
+        <f t="shared" si="6"/>
+        <v>52.229201760000002</v>
+      </c>
+      <c r="L37" s="48">
+        <f t="shared" si="7"/>
+        <v>46.813847803810269</v>
+      </c>
+      <c r="M37" s="19">
+        <v>0.52000400000000002</v>
+      </c>
+      <c r="N37">
+        <v>2.68</v>
+      </c>
+      <c r="O37" s="28">
+        <v>5.6366754364629776E-2</v>
+      </c>
+      <c r="P37" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q37" s="43">
+        <v>6.0392103392567247</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="37"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B40" s="38"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
atualização em código do KPI, onde foi pré-adicionado um código de intervalos na mobilidade elétrica
</commit_message>
<xml_diff>
--- a/kpis_energia_por_unidade.xlsx
+++ b/kpis_energia_por_unidade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayrton\Documents\GitHub\atnee\kpis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD920232-9788-4A16-A448-40A02F565869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E58E1-4F84-4A2F-BF83-4C693C54D193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="0" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>Tempo</t>
   </si>
   <si>
-    <t>Mês</t>
-  </si>
-  <si>
     <t>km</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Economia</t>
+  </si>
+  <si>
+    <t>Mês</t>
   </si>
 </sst>
 </file>
@@ -293,7 +293,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -393,9 +393,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,12 +424,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Moeda" xfId="3" builtinId="4"/>
@@ -441,14 +438,7 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
     <cellStyle name="Vírgula 4" xfId="2" xr:uid="{7CBFA859-85D8-46D5-A762-F87CB82252FC}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -734,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54:M54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2307,7 +2297,7 @@
       <c r="L38" s="22">
         <v>0.54781599999999997</v>
       </c>
-      <c r="M38" s="53">
+      <c r="M38" s="27">
         <v>0.41635942812446686</v>
       </c>
     </row>
@@ -2348,7 +2338,7 @@
       <c r="L39" s="22">
         <v>0.55078700000000003</v>
       </c>
-      <c r="M39" s="53">
+      <c r="M39" s="27">
         <v>0.37498332200554002</v>
       </c>
     </row>
@@ -2389,7 +2379,7 @@
       <c r="L40" s="23">
         <v>0.546991</v>
       </c>
-      <c r="M40" s="53">
+      <c r="M40" s="27">
         <v>0.27790975910056098</v>
       </c>
     </row>
@@ -2430,7 +2420,7 @@
       <c r="L41" s="23">
         <v>0.53952599999999995</v>
       </c>
-      <c r="M41" s="53">
+      <c r="M41" s="27">
         <v>0.194634416756858</v>
       </c>
     </row>
@@ -2471,7 +2461,7 @@
       <c r="L42" s="23">
         <v>0.54575600000000002</v>
       </c>
-      <c r="M42" s="53">
+      <c r="M42" s="27">
         <v>0.28342692993865498</v>
       </c>
     </row>
@@ -2512,7 +2502,7 @@
       <c r="L43" s="23">
         <v>0.556674</v>
       </c>
-      <c r="M43" s="53">
+      <c r="M43" s="27">
         <v>0.36478268557543064</v>
       </c>
     </row>
@@ -2553,7 +2543,7 @@
       <c r="L44" s="23">
         <v>0.56105400000000005</v>
       </c>
-      <c r="M44" s="53">
+      <c r="M44" s="27">
         <v>0.55029254581602527</v>
       </c>
     </row>
@@ -2594,7 +2584,7 @@
       <c r="L45" s="23">
         <v>0.52071100000000003</v>
       </c>
-      <c r="M45" s="53">
+      <c r="M45" s="27">
         <v>0.60146943007921028</v>
       </c>
     </row>
@@ -2635,7 +2625,7 @@
       <c r="L46" s="23">
         <v>0.50722400000000001</v>
       </c>
-      <c r="M46" s="53">
+      <c r="M46" s="27">
         <v>0.60540367356437397</v>
       </c>
     </row>
@@ -2676,7 +2666,7 @@
       <c r="L47" s="19">
         <v>0.51760300000000004</v>
       </c>
-      <c r="M47" s="53">
+      <c r="M47" s="27">
         <v>0.64768070653495458</v>
       </c>
     </row>
@@ -2717,7 +2707,7 @@
       <c r="L48" s="19">
         <v>0.51696500000000001</v>
       </c>
-      <c r="M48" s="53">
+      <c r="M48" s="27">
         <v>0.5523540164322871</v>
       </c>
     </row>
@@ -2758,7 +2748,7 @@
       <c r="L49" s="19">
         <v>0.52000400000000002</v>
       </c>
-      <c r="M49" s="53">
+      <c r="M49" s="27">
         <v>0.49778509841850888</v>
       </c>
     </row>
@@ -2766,10 +2756,10 @@
       <c r="A50" s="10">
         <v>45658</v>
       </c>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="55"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
       <c r="F50" s="15">
         <v>1999.6</v>
       </c>
@@ -2791,7 +2781,7 @@
       <c r="L50" s="19">
         <v>0.50707400000000002</v>
       </c>
-      <c r="M50" s="53">
+      <c r="M50" s="27">
         <v>0.49778509841850888</v>
       </c>
     </row>
@@ -2799,11 +2789,11 @@
       <c r="A51" s="10">
         <v>45689</v>
       </c>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
       <c r="G51" s="15">
         <v>0</v>
       </c>
@@ -2822,7 +2812,7 @@
       <c r="L51" s="19">
         <v>0.503965</v>
       </c>
-      <c r="M51" s="53">
+      <c r="M51" s="27">
         <v>0.49778509841850888</v>
       </c>
     </row>
@@ -2830,11 +2820,11 @@
       <c r="A52" s="10">
         <v>45717</v>
       </c>
-      <c r="B52" s="55"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
       <c r="G52" s="15">
         <v>0</v>
       </c>
@@ -2850,10 +2840,10 @@
       <c r="K52" s="15">
         <v>5121.6000000000004</v>
       </c>
-      <c r="L52" s="54">
+      <c r="L52" s="52">
         <v>0.503965</v>
       </c>
-      <c r="M52" s="53">
+      <c r="M52" s="27">
         <v>0.49778509841850888</v>
       </c>
     </row>
@@ -2861,11 +2851,11 @@
       <c r="A53" s="10">
         <v>45748</v>
       </c>
-      <c r="B53" s="55"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
       <c r="G53" s="15">
         <v>385</v>
       </c>
@@ -2881,10 +2871,10 @@
       <c r="K53" s="15">
         <v>4953.3999999999996</v>
       </c>
-      <c r="L53" s="54">
+      <c r="L53" s="52">
         <v>0.503965</v>
       </c>
-      <c r="M53" s="53">
+      <c r="M53" s="27">
         <v>0.49778509841850888</v>
       </c>
     </row>
@@ -2892,18 +2882,18 @@
       <c r="A54" s="10">
         <v>45778</v>
       </c>
-      <c r="B54" s="56"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="56"/>
-      <c r="I54" s="56"/>
-      <c r="J54" s="56"/>
-      <c r="K54" s="56"/>
-      <c r="L54" s="56"/>
-      <c r="M54" s="56"/>
+      <c r="B54" s="54"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="54"/>
+      <c r="I54" s="54"/>
+      <c r="J54" s="54"/>
+      <c r="K54" s="54"/>
+      <c r="L54" s="54"/>
+      <c r="M54" s="54"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B49">
@@ -2967,9 +2957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AC82A9-1A92-44C2-9406-62A85459B06F}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2990,69 +2978,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="C1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="E1" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="42" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="39">
+      <c r="A2" s="55">
         <v>44562</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="39">
         <v>2652.18</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="39">
         <v>2886.84</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="39">
         <v>18</v>
       </c>
       <c r="E2">
@@ -3067,7 +3055,7 @@
         <f>(E2-F2)/1000</f>
         <v>2.6489973839999998</v>
       </c>
-      <c r="H2" s="52">
+      <c r="H2" s="51">
         <f>((E2-F2)/E2)*100</f>
         <v>93.171641791044777</v>
       </c>
@@ -3075,15 +3063,15 @@
         <f t="shared" ref="I2:I37" si="2">B2/P2</f>
         <v>1060.8719999999998</v>
       </c>
-      <c r="J2" s="47">
+      <c r="J2" s="46">
         <f>I2*Q2</f>
         <v>5824.1872799999992</v>
       </c>
-      <c r="K2" s="47">
+      <c r="K2" s="46">
         <f>C2*M2</f>
         <v>1159.56857016</v>
       </c>
-      <c r="L2" s="47">
+      <c r="L2" s="46">
         <f>J2-K2</f>
         <v>4664.6187098399987</v>
       </c>
@@ -3096,24 +3084,24 @@
       <c r="O2" s="27">
         <v>7.3200000000000001E-2</v>
       </c>
-      <c r="P2" s="44">
+      <c r="P2" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q2" s="42">
+      <c r="Q2" s="41">
         <v>5.49</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="39">
+      <c r="A3" s="55">
         <v>44593</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="39">
         <v>601.24</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="39">
         <v>628.55999999999995</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="39">
         <v>4</v>
       </c>
       <c r="E3">
@@ -3128,7 +3116,7 @@
         <f t="shared" ref="G3:G37" si="3">(E3-F3)/1000</f>
         <v>0.61431454045627476</v>
       </c>
-      <c r="H3" s="52">
+      <c r="H3" s="51">
         <f t="shared" ref="H3:H37" si="4">((E3-F3)/E3)*100</f>
         <v>95.31212305145776</v>
       </c>
@@ -3136,15 +3124,15 @@
         <f t="shared" si="2"/>
         <v>240.49600000000001</v>
       </c>
-      <c r="J3" s="47">
+      <c r="J3" s="46">
         <f t="shared" ref="J3:J37" si="5">I3*Q3</f>
         <v>1346.7775999999999</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="46">
         <f t="shared" ref="K3:K37" si="6">C3*M3</f>
         <v>259.59590856</v>
       </c>
-      <c r="L3" s="47">
+      <c r="L3" s="46">
         <f t="shared" ref="L3:L37" si="7">J3-K3</f>
         <v>1087.1816914399999</v>
       </c>
@@ -3157,24 +3145,24 @@
       <c r="O3" s="27">
         <v>5.0254040888372771E-2</v>
       </c>
-      <c r="P3" s="44">
+      <c r="P3" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q3" s="42">
+      <c r="Q3" s="41">
         <v>5.6</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="39">
+      <c r="A4" s="55">
         <v>44621</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="39">
         <v>3128.78</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="39">
         <v>3657.96</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="39">
         <v>21</v>
       </c>
       <c r="E4">
@@ -3189,7 +3177,7 @@
         <f t="shared" si="3"/>
         <v>3.2269763058729923</v>
       </c>
-      <c r="H4" s="52">
+      <c r="H4" s="51">
         <f t="shared" si="4"/>
         <v>96.211273764835894</v>
       </c>
@@ -3197,15 +3185,15 @@
         <f t="shared" si="2"/>
         <v>1251.5120000000002</v>
       </c>
-      <c r="J4" s="47">
+      <c r="J4" s="46">
         <f t="shared" si="5"/>
         <v>7846.9802400000008</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="46">
         <f t="shared" si="6"/>
         <v>1466.5310334000001</v>
       </c>
-      <c r="L4" s="47">
+      <c r="L4" s="46">
         <f t="shared" si="7"/>
         <v>6380.4492066000003</v>
       </c>
@@ -3218,24 +3206,24 @@
       <c r="O4" s="27">
         <v>4.0615145240959265E-2</v>
       </c>
-      <c r="P4" s="44">
+      <c r="P4" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q4" s="42">
+      <c r="Q4" s="41">
         <v>6.27</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="39">
+      <c r="A5" s="55">
         <v>44652</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="39">
         <v>2418</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="39">
         <v>3116.88</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="39">
         <v>16</v>
       </c>
       <c r="E5">
@@ -3250,7 +3238,7 @@
         <f t="shared" si="3"/>
         <v>2.5398958650626264</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="51">
         <f t="shared" si="4"/>
         <v>97.986180491101635</v>
       </c>
@@ -3258,15 +3246,15 @@
         <f t="shared" si="2"/>
         <v>967.2</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="46">
         <f t="shared" si="5"/>
         <v>6393.1920000000009</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="46">
         <f t="shared" si="6"/>
         <v>1273.1083372799999</v>
       </c>
-      <c r="L5" s="47">
+      <c r="L5" s="46">
         <f t="shared" si="7"/>
         <v>5120.0836627200006</v>
       </c>
@@ -3279,24 +3267,24 @@
       <c r="O5" s="27">
         <v>2.1588145135390389E-2</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q5" s="42">
+      <c r="Q5" s="41">
         <v>6.61</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
+      <c r="A6" s="55">
         <v>44682</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="39">
         <v>3318.2</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="39">
         <v>4147.2</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="39">
         <v>22</v>
       </c>
       <c r="E6">
@@ -3311,7 +3299,7 @@
         <f t="shared" si="3"/>
         <v>3.4641170888604771</v>
       </c>
-      <c r="H6" s="52">
+      <c r="H6" s="51">
         <f t="shared" si="4"/>
         <v>97.385706354811958</v>
       </c>
@@ -3319,15 +3307,15 @@
         <f t="shared" si="2"/>
         <v>1327.28</v>
       </c>
-      <c r="J6" s="47">
+      <c r="J6" s="46">
         <f t="shared" si="5"/>
         <v>9105.140800000001</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="46">
         <f t="shared" si="6"/>
         <v>1718.9356031999998</v>
       </c>
-      <c r="L6" s="47">
+      <c r="L6" s="46">
         <f t="shared" si="7"/>
         <v>7386.2051968000014</v>
       </c>
@@ -3340,24 +3328,24 @@
       <c r="O6" s="27">
         <v>2.8025227876415777E-2</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q6" s="42">
+      <c r="Q6" s="41">
         <v>6.86</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
+      <c r="A7" s="55">
         <v>44713</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="39">
         <v>3167.37</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="39">
         <v>3962.52</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="39">
         <v>21</v>
       </c>
       <c r="E7">
@@ -3372,7 +3360,7 @@
         <f t="shared" si="3"/>
         <v>3.255864401508358</v>
       </c>
-      <c r="H7" s="52">
+      <c r="H7" s="51">
         <f t="shared" si="4"/>
         <v>95.889868935601399</v>
       </c>
@@ -3380,15 +3368,15 @@
         <f t="shared" si="2"/>
         <v>1266.9479999999999</v>
       </c>
-      <c r="J7" s="47">
+      <c r="J7" s="46">
         <f t="shared" si="5"/>
         <v>9122.025599999999</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="46">
         <f t="shared" si="6"/>
         <v>1623.02441688</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="46">
         <f t="shared" si="7"/>
         <v>7499.001183119999</v>
       </c>
@@ -3401,24 +3389,24 @@
       <c r="O7" s="27">
         <v>4.4060605010353047E-2</v>
       </c>
-      <c r="P7" s="44">
+      <c r="P7" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q7" s="42">
+      <c r="Q7" s="41">
         <v>7.2</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="39">
+      <c r="A8" s="55">
         <v>44743</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="39">
         <v>2977.96</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="39">
         <v>3508.92</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="39">
         <v>20</v>
       </c>
       <c r="E8">
@@ -3433,7 +3421,7 @@
         <f t="shared" si="3"/>
         <v>3.0676986584203454</v>
       </c>
-      <c r="H8" s="52">
+      <c r="H8" s="51">
         <f t="shared" si="4"/>
         <v>96.094614980981461</v>
       </c>
@@ -3441,15 +3429,15 @@
         <f t="shared" si="2"/>
         <v>1191.184</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="46">
         <f t="shared" si="5"/>
         <v>8850.49712</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="46">
         <f t="shared" si="6"/>
         <v>1319.0732063999999</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="46">
         <f t="shared" si="7"/>
         <v>7531.4239135999997</v>
       </c>
@@ -3462,24 +3450,24 @@
       <c r="O8" s="27">
         <v>4.1865727403878748E-2</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q8" s="42">
+      <c r="Q8" s="41">
         <v>7.43</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
+      <c r="A9" s="55">
         <v>44774</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="39">
         <v>2991.78</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="39">
         <v>3926.88</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="39">
         <v>20</v>
       </c>
       <c r="E9">
@@ -3494,7 +3482,7 @@
         <f t="shared" si="3"/>
         <v>3.0704216961152406</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="51">
         <f t="shared" si="4"/>
         <v>95.735627064526213</v>
       </c>
@@ -3502,15 +3490,15 @@
         <f t="shared" si="2"/>
         <v>1196.712</v>
       </c>
-      <c r="J9" s="47">
+      <c r="J9" s="46">
         <f t="shared" si="5"/>
         <v>8484.6880799999999</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="46">
         <f t="shared" si="6"/>
         <v>1620.8236468800001</v>
       </c>
-      <c r="L9" s="47">
+      <c r="L9" s="46">
         <f t="shared" si="7"/>
         <v>6863.8644331199994</v>
       </c>
@@ -3523,24 +3511,24 @@
       <c r="O9" s="27">
         <v>4.5714077868278892E-2</v>
       </c>
-      <c r="P9" s="44">
+      <c r="P9" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q9" s="42">
+      <c r="Q9" s="41">
         <v>7.09</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
+      <c r="A10" s="55">
         <v>44805</v>
       </c>
-      <c r="B10" s="40">
+      <c r="B10" s="39">
         <v>3177.56</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="39">
         <v>4228.2</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="39">
         <v>21</v>
       </c>
       <c r="E10">
@@ -3555,7 +3543,7 @@
         <f t="shared" si="3"/>
         <v>3.2503687043037472</v>
       </c>
-      <c r="H10" s="52">
+      <c r="H10" s="51">
         <f t="shared" si="4"/>
         <v>95.421026148752546</v>
       </c>
@@ -3563,15 +3551,15 @@
         <f t="shared" si="2"/>
         <v>1271.0239999999999</v>
       </c>
-      <c r="J10" s="47">
+      <c r="J10" s="46">
         <f t="shared" si="5"/>
         <v>8693.8041599999997</v>
       </c>
-      <c r="K10" s="47">
+      <c r="K10" s="46">
         <f t="shared" si="6"/>
         <v>1758.4111313999999</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="46">
         <f t="shared" si="7"/>
         <v>6935.3930285999995</v>
       </c>
@@ -3584,24 +3572,24 @@
       <c r="O10" s="27">
         <v>4.9086599685372614E-2</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q10" s="42">
+      <c r="Q10" s="41">
         <v>6.84</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="A11" s="55">
         <v>44835</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="39">
         <v>2560.7199999999998</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="39">
         <v>3593.16</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="39">
         <v>17</v>
       </c>
       <c r="E11">
@@ -3616,7 +3604,7 @@
         <f t="shared" si="3"/>
         <v>2.6244176018694425</v>
       </c>
-      <c r="H11" s="52">
+      <c r="H11" s="51">
         <f t="shared" si="4"/>
         <v>95.603999969248477</v>
       </c>
@@ -3624,15 +3612,15 @@
         <f t="shared" si="2"/>
         <v>1024.288</v>
       </c>
-      <c r="J11" s="47">
+      <c r="J11" s="46">
         <f t="shared" si="5"/>
         <v>6627.14336</v>
       </c>
-      <c r="K11" s="47">
+      <c r="K11" s="46">
         <f t="shared" si="6"/>
         <v>1486.1094170399999</v>
       </c>
-      <c r="L11" s="47">
+      <c r="L11" s="46">
         <f t="shared" si="7"/>
         <v>5141.0339429599999</v>
       </c>
@@ -3645,24 +3633,24 @@
       <c r="O11" s="27">
         <v>4.7125120329656413E-2</v>
       </c>
-      <c r="P11" s="44">
+      <c r="P11" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q11" s="42">
+      <c r="Q11" s="41">
         <v>6.47</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="A12" s="55">
         <v>44866</v>
       </c>
-      <c r="B12" s="40">
+      <c r="B12" s="39">
         <v>2304.3200000000002</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="39">
         <v>2928.96</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="39">
         <v>15</v>
       </c>
       <c r="E12">
@@ -3677,7 +3665,7 @@
         <f t="shared" si="3"/>
         <v>2.3774973484682804</v>
       </c>
-      <c r="H12" s="52">
+      <c r="H12" s="51">
         <f t="shared" si="4"/>
         <v>96.245950681126587</v>
       </c>
@@ -3685,15 +3673,15 @@
         <f t="shared" si="2"/>
         <v>921.72800000000007</v>
       </c>
-      <c r="J12" s="47">
+      <c r="J12" s="46">
         <f t="shared" si="5"/>
         <v>5991.232</v>
       </c>
-      <c r="K12" s="47">
+      <c r="K12" s="46">
         <f t="shared" si="6"/>
         <v>1204.1598931199999</v>
       </c>
-      <c r="L12" s="47">
+      <c r="L12" s="46">
         <f t="shared" si="7"/>
         <v>4787.0721068800003</v>
       </c>
@@ -3706,24 +3694,24 @@
       <c r="O12" s="27">
         <v>4.0243408698322984E-2</v>
       </c>
-      <c r="P12" s="44">
+      <c r="P12" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q12" s="42">
+      <c r="Q12" s="41">
         <v>6.5</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="39">
+      <c r="A13" s="55">
         <v>44896</v>
       </c>
-      <c r="B13" s="40">
-        <v>0</v>
-      </c>
-      <c r="C13" s="40">
-        <v>0</v>
-      </c>
-      <c r="D13" s="40">
+      <c r="B13" s="39">
+        <v>0</v>
+      </c>
+      <c r="C13" s="39">
+        <v>0</v>
+      </c>
+      <c r="D13" s="39">
         <v>0</v>
       </c>
       <c r="E13">
@@ -3738,7 +3726,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H13" s="52" t="e">
+      <c r="H13" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -3746,15 +3734,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="47">
+      <c r="J13" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K13" s="47">
+      <c r="K13" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L13" s="47">
+      <c r="L13" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3767,24 +3755,24 @@
       <c r="O13" s="27">
         <v>2.9368484258302584E-2</v>
       </c>
-      <c r="P13" s="44">
+      <c r="P13" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q13" s="42">
+      <c r="Q13" s="41">
         <v>6.35</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="A14" s="55">
         <v>44927</v>
       </c>
-      <c r="B14" s="40">
-        <v>0</v>
-      </c>
-      <c r="C14" s="40">
-        <v>0</v>
-      </c>
-      <c r="D14" s="40">
+      <c r="B14" s="39">
+        <v>0</v>
+      </c>
+      <c r="C14" s="39">
+        <v>0</v>
+      </c>
+      <c r="D14" s="39">
         <v>0</v>
       </c>
       <c r="E14">
@@ -3799,7 +3787,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H14" s="52" t="e">
+      <c r="H14" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -3807,15 +3795,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K14" s="47">
+      <c r="K14" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L14" s="47">
+      <c r="L14" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3828,24 +3816,24 @@
       <c r="O14" s="27">
         <v>2.9173607327091757E-2</v>
       </c>
-      <c r="P14" s="44">
+      <c r="P14" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q14" s="42">
+      <c r="Q14" s="41">
         <v>6.3</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="39">
+      <c r="A15" s="55">
         <v>44958</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="39">
         <v>1013.4349999999977</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="39">
         <v>774.36</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="39">
         <v>5</v>
       </c>
       <c r="E15">
@@ -3860,7 +3848,7 @@
         <f t="shared" si="3"/>
         <v>1.0623091450036797</v>
       </c>
-      <c r="H15" s="52">
+      <c r="H15" s="51">
         <f t="shared" si="4"/>
         <v>97.782297169954688</v>
       </c>
@@ -3868,15 +3856,15 @@
         <f t="shared" si="2"/>
         <v>405.37399999999906</v>
       </c>
-      <c r="J15" s="47">
+      <c r="J15" s="46">
         <f t="shared" si="5"/>
         <v>2456.5664399999941</v>
       </c>
-      <c r="K15" s="47">
+      <c r="K15" s="46">
         <f t="shared" si="6"/>
         <v>329.36473368000003</v>
       </c>
-      <c r="L15" s="47">
+      <c r="L15" s="46">
         <f t="shared" si="7"/>
         <v>2127.2017063199942</v>
       </c>
@@ -3889,24 +3877,24 @@
       <c r="O15" s="27">
         <v>2.3773774338085845E-2</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q15" s="42">
+      <c r="Q15" s="41">
         <v>6.06</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="39">
+      <c r="A16" s="55">
         <v>44986</v>
       </c>
-      <c r="B16" s="40">
+      <c r="B16" s="39">
         <v>272</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="39">
         <v>463.32</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="39">
         <v>3</v>
       </c>
       <c r="E16">
@@ -3921,7 +3909,7 @@
         <f t="shared" si="3"/>
         <v>0.2835401514721208</v>
       </c>
-      <c r="H16" s="52">
+      <c r="H16" s="51">
         <f t="shared" si="4"/>
         <v>97.24132718946197</v>
       </c>
@@ -3929,15 +3917,15 @@
         <f t="shared" si="2"/>
         <v>108.8</v>
       </c>
-      <c r="J16" s="47">
+      <c r="J16" s="46">
         <f t="shared" si="5"/>
         <v>638.65599999999995</v>
       </c>
-      <c r="K16" s="47">
+      <c r="K16" s="46">
         <f t="shared" si="6"/>
         <v>198.13462812</v>
       </c>
-      <c r="L16" s="47">
+      <c r="L16" s="46">
         <f t="shared" si="7"/>
         <v>440.52137187999995</v>
       </c>
@@ -3950,24 +3938,24 @@
       <c r="O16" s="27">
         <v>2.9572972528967699E-2</v>
       </c>
-      <c r="P16" s="44">
+      <c r="P16" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q16" s="42">
+      <c r="Q16" s="41">
         <v>5.87</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="39">
+      <c r="A17" s="55">
         <v>45017</v>
       </c>
-      <c r="B17" s="40">
-        <v>0</v>
-      </c>
-      <c r="C17" s="40">
-        <v>0</v>
-      </c>
-      <c r="D17" s="40">
+      <c r="B17" s="39">
+        <v>0</v>
+      </c>
+      <c r="C17" s="39">
+        <v>0</v>
+      </c>
+      <c r="D17" s="39">
         <v>0</v>
       </c>
       <c r="E17">
@@ -3982,7 +3970,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H17" s="52" t="e">
+      <c r="H17" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -3990,15 +3978,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K17" s="47">
+      <c r="K17" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L17" s="47">
+      <c r="L17" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4011,24 +3999,24 @@
       <c r="O17" s="27">
         <v>3.40267536628742E-2</v>
       </c>
-      <c r="P17" s="44">
+      <c r="P17" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q17" s="42">
+      <c r="Q17" s="41">
         <v>5.74</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
+      <c r="A18" s="55">
         <v>45047</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="39">
         <v>147</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="39">
         <v>142.56</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="39">
         <v>1</v>
       </c>
       <c r="E18">
@@ -4043,7 +4031,7 @@
         <f t="shared" si="3"/>
         <v>0.15324591488702163</v>
       </c>
-      <c r="H18" s="52">
+      <c r="H18" s="51">
         <f t="shared" si="4"/>
         <v>97.24712844389127</v>
       </c>
@@ -4051,15 +4039,15 @@
         <f t="shared" si="2"/>
         <v>58.8</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="46">
         <f t="shared" si="5"/>
         <v>316.34399999999999</v>
       </c>
-      <c r="K18" s="47">
+      <c r="K18" s="46">
         <f t="shared" si="6"/>
         <v>59.961021119999998</v>
       </c>
-      <c r="L18" s="47">
+      <c r="L18" s="46">
         <f t="shared" si="7"/>
         <v>256.38297888</v>
       </c>
@@ -4072,24 +4060,24 @@
       <c r="O18" s="27">
         <v>2.9510783081485501E-2</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q18" s="42">
+      <c r="Q18" s="41">
         <v>5.38</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="39">
+      <c r="A19" s="55">
         <v>45078</v>
       </c>
-      <c r="B19" s="40">
-        <v>0</v>
-      </c>
-      <c r="C19" s="40">
-        <v>0</v>
-      </c>
-      <c r="D19" s="40">
+      <c r="B19" s="39">
+        <v>0</v>
+      </c>
+      <c r="C19" s="39">
+        <v>0</v>
+      </c>
+      <c r="D19" s="39">
         <v>0</v>
       </c>
       <c r="E19">
@@ -4104,7 +4092,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H19" s="52" t="e">
+      <c r="H19" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4112,15 +4100,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K19" s="47">
+      <c r="K19" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L19" s="47">
+      <c r="L19" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4133,24 +4121,24 @@
       <c r="O19" s="27">
         <v>5.2787803573402799E-2</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q19" s="42">
+      <c r="Q19" s="41">
         <v>5.05</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="39">
+      <c r="A20" s="55">
         <v>45108</v>
       </c>
-      <c r="B20" s="40">
-        <v>0</v>
-      </c>
-      <c r="C20" s="40">
-        <v>0</v>
-      </c>
-      <c r="D20" s="40">
+      <c r="B20" s="39">
+        <v>0</v>
+      </c>
+      <c r="C20" s="39">
+        <v>0</v>
+      </c>
+      <c r="D20" s="39">
         <v>0</v>
       </c>
       <c r="E20">
@@ -4165,7 +4153,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H20" s="52" t="e">
+      <c r="H20" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4173,15 +4161,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J20" s="47">
+      <c r="J20" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K20" s="47">
+      <c r="K20" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L20" s="47">
+      <c r="L20" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4194,24 +4182,24 @@
       <c r="O20" s="27">
         <v>4.9510010162503372E-2</v>
       </c>
-      <c r="P20" s="44">
+      <c r="P20" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q20" s="42">
+      <c r="Q20" s="41">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
+      <c r="A21" s="55">
         <v>45139</v>
       </c>
-      <c r="B21" s="40">
+      <c r="B21" s="39">
         <v>162</v>
       </c>
-      <c r="C21" s="40">
+      <c r="C21" s="39">
         <v>142.55999999999995</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="39">
         <v>4</v>
       </c>
       <c r="E21">
@@ -4226,7 +4214,7 @@
         <f t="shared" si="3"/>
         <v>0.16687605953310905</v>
       </c>
-      <c r="H21" s="52">
+      <c r="H21" s="51">
         <f t="shared" si="4"/>
         <v>96.091337026159152</v>
       </c>
@@ -4234,15 +4222,15 @@
         <f t="shared" si="2"/>
         <v>64.8</v>
       </c>
-      <c r="J21" s="47">
+      <c r="J21" s="46">
         <f t="shared" si="5"/>
         <v>358.34399999999999</v>
       </c>
-      <c r="K21" s="47">
+      <c r="K21" s="46">
         <f t="shared" si="6"/>
         <v>70.359062399999971</v>
       </c>
-      <c r="L21" s="47">
+      <c r="L21" s="46">
         <f t="shared" si="7"/>
         <v>287.98493760000002</v>
       </c>
@@ -4255,24 +4243,24 @@
       <c r="O21" s="27">
         <v>4.1900867079573897E-2</v>
       </c>
-      <c r="P21" s="44">
+      <c r="P21" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q21" s="42">
+      <c r="Q21" s="41">
         <v>5.53</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="A22" s="55">
         <v>45170</v>
       </c>
-      <c r="B22" s="40">
-        <v>0</v>
-      </c>
-      <c r="C22" s="40">
-        <v>0</v>
-      </c>
-      <c r="D22" s="40">
+      <c r="B22" s="39">
+        <v>0</v>
+      </c>
+      <c r="C22" s="39">
+        <v>0</v>
+      </c>
+      <c r="D22" s="39">
         <v>0</v>
       </c>
       <c r="E22">
@@ -4287,7 +4275,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H22" s="52" t="e">
+      <c r="H22" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4295,15 +4283,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="47">
+      <c r="J22" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K22" s="47">
+      <c r="K22" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L22" s="47">
+      <c r="L22" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4316,24 +4304,24 @@
       <c r="O22" s="27">
         <v>3.4334475892947448E-2</v>
       </c>
-      <c r="P22" s="44">
+      <c r="P22" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q22" s="42">
+      <c r="Q22" s="41">
         <v>6.07</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
+      <c r="A23" s="55">
         <v>45200</v>
       </c>
-      <c r="B23" s="40">
-        <v>0</v>
-      </c>
-      <c r="C23" s="40">
-        <v>0</v>
-      </c>
-      <c r="D23" s="40">
+      <c r="B23" s="39">
+        <v>0</v>
+      </c>
+      <c r="C23" s="39">
+        <v>0</v>
+      </c>
+      <c r="D23" s="39">
         <v>0</v>
       </c>
       <c r="E23">
@@ -4348,7 +4336,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H23" s="52" t="e">
+      <c r="H23" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4356,15 +4344,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="47">
+      <c r="J23" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K23" s="47">
+      <c r="K23" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L23" s="47">
+      <c r="L23" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4377,24 +4365,24 @@
       <c r="O23" s="27">
         <v>3.8729598739869808E-2</v>
       </c>
-      <c r="P23" s="44">
+      <c r="P23" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q23" s="42">
+      <c r="Q23" s="41">
         <v>6.08</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="39">
+      <c r="A24" s="55">
         <v>45231</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="39">
         <v>63</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="39">
         <v>90</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="39">
         <v>2</v>
       </c>
       <c r="E24">
@@ -4409,7 +4397,7 @@
         <f t="shared" si="3"/>
         <v>6.4201682639637089E-2</v>
       </c>
-      <c r="H24" s="52">
+      <c r="H24" s="51">
         <f t="shared" si="4"/>
         <v>95.062903695269313</v>
       </c>
@@ -4417,15 +4405,15 @@
         <f t="shared" si="2"/>
         <v>25.2</v>
       </c>
-      <c r="J24" s="47">
+      <c r="J24" s="46">
         <f t="shared" si="5"/>
         <v>153.21600000000001</v>
       </c>
-      <c r="K24" s="47">
+      <c r="K24" s="46">
         <f t="shared" si="6"/>
         <v>48.633030000000005</v>
       </c>
-      <c r="L24" s="47">
+      <c r="L24" s="46">
         <f t="shared" si="7"/>
         <v>104.58297</v>
       </c>
@@ -4438,24 +4426,24 @@
       <c r="O24" s="27">
         <v>5.2925672386713071E-2</v>
       </c>
-      <c r="P24" s="44">
+      <c r="P24" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q24" s="42">
+      <c r="Q24" s="41">
         <v>6.08</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="39">
+      <c r="A25" s="55">
         <v>45261</v>
       </c>
-      <c r="B25" s="40">
-        <v>0</v>
-      </c>
-      <c r="C25" s="40">
-        <v>0</v>
-      </c>
-      <c r="D25" s="40">
+      <c r="B25" s="39">
+        <v>0</v>
+      </c>
+      <c r="C25" s="39">
+        <v>0</v>
+      </c>
+      <c r="D25" s="39">
         <v>0</v>
       </c>
       <c r="E25">
@@ -4470,7 +4458,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H25" s="52" t="e">
+      <c r="H25" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4478,15 +4466,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="47">
+      <c r="J25" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K25" s="47">
+      <c r="K25" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L25" s="47">
+      <c r="L25" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4499,24 +4487,24 @@
       <c r="O25" s="27">
         <v>4.586845854173565E-2</v>
       </c>
-      <c r="P25" s="44">
+      <c r="P25" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q25" s="42">
+      <c r="Q25" s="41">
         <v>5.94</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="39">
+      <c r="A26" s="55">
         <v>45292</v>
       </c>
-      <c r="B26" s="41">
+      <c r="B26" s="40">
         <v>1260</v>
       </c>
-      <c r="C26" s="40">
+      <c r="C26" s="39">
         <v>1487.16</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="39">
         <v>8</v>
       </c>
       <c r="E26">
@@ -4531,7 +4519,7 @@
         <f t="shared" si="3"/>
         <v>1.2976738149702167</v>
       </c>
-      <c r="H26" s="52">
+      <c r="H26" s="51">
         <f t="shared" si="4"/>
         <v>96.072747495425887</v>
       </c>
@@ -4539,15 +4527,15 @@
         <f t="shared" si="2"/>
         <v>504</v>
       </c>
-      <c r="J26" s="47">
+      <c r="J26" s="46">
         <f t="shared" si="5"/>
         <v>2963.52</v>
       </c>
-      <c r="K26" s="47">
+      <c r="K26" s="46">
         <f t="shared" si="6"/>
         <v>814.69004256000005</v>
       </c>
-      <c r="L26" s="47">
+      <c r="L26" s="46">
         <f t="shared" si="7"/>
         <v>2148.8299574399998</v>
       </c>
@@ -4560,24 +4548,24 @@
       <c r="O26" s="27">
         <v>4.2100146849034403E-2</v>
       </c>
-      <c r="P26" s="44">
+      <c r="P26" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q26" s="42">
+      <c r="Q26" s="41">
         <v>5.88</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="39">
+      <c r="A27" s="55">
         <v>45323</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="39">
         <v>213</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="39">
         <v>249.48</v>
       </c>
-      <c r="D27" s="40">
+      <c r="D27" s="39">
         <v>1</v>
       </c>
       <c r="E27">
@@ -4592,7 +4580,7 @@
         <f t="shared" si="3"/>
         <v>0.22033227960658966</v>
       </c>
-      <c r="H27" s="52">
+      <c r="H27" s="51">
         <f t="shared" si="4"/>
         <v>96.494761932673626</v>
       </c>
@@ -4600,15 +4588,15 @@
         <f t="shared" si="2"/>
         <v>85.2</v>
       </c>
-      <c r="J27" s="47">
+      <c r="J27" s="46">
         <f t="shared" si="5"/>
         <v>500.976</v>
       </c>
-      <c r="K27" s="47">
+      <c r="K27" s="46">
         <f t="shared" si="6"/>
         <v>137.41034076</v>
       </c>
-      <c r="L27" s="47">
+      <c r="L27" s="46">
         <f t="shared" si="7"/>
         <v>363.56565924</v>
       </c>
@@ -4621,24 +4609,24 @@
       <c r="O27" s="27">
         <v>3.7576152081738791E-2</v>
       </c>
-      <c r="P27" s="44">
+      <c r="P27" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q27" s="42">
+      <c r="Q27" s="41">
         <v>5.88</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="39">
+      <c r="A28" s="55">
         <v>45352</v>
       </c>
-      <c r="B28" s="40">
-        <v>0</v>
-      </c>
-      <c r="C28" s="40">
-        <v>0</v>
-      </c>
-      <c r="D28" s="40">
+      <c r="B28" s="39">
+        <v>0</v>
+      </c>
+      <c r="C28" s="39">
+        <v>0</v>
+      </c>
+      <c r="D28" s="39">
         <v>0</v>
       </c>
       <c r="E28">
@@ -4653,7 +4641,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H28" s="52" t="e">
+      <c r="H28" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4661,15 +4649,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28" s="47">
+      <c r="J28" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K28" s="47">
+      <c r="K28" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L28" s="47">
+      <c r="L28" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4682,24 +4670,24 @@
       <c r="O28" s="27">
         <v>2.7790975910056099E-2</v>
       </c>
-      <c r="P28" s="44">
+      <c r="P28" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q28" s="42">
+      <c r="Q28" s="41">
         <v>5.1933031268038796</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="39">
+      <c r="A29" s="55">
         <v>45383</v>
       </c>
-      <c r="B29" s="40">
-        <v>0</v>
-      </c>
-      <c r="C29" s="40">
-        <v>0</v>
-      </c>
-      <c r="D29" s="40">
+      <c r="B29" s="39">
+        <v>0</v>
+      </c>
+      <c r="C29" s="39">
+        <v>0</v>
+      </c>
+      <c r="D29" s="39">
         <v>0</v>
       </c>
       <c r="E29">
@@ -4714,7 +4702,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H29" s="52" t="e">
+      <c r="H29" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4722,15 +4710,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J29" s="47">
+      <c r="J29" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K29" s="47">
+      <c r="K29" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L29" s="47">
+      <c r="L29" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4743,24 +4731,24 @@
       <c r="O29" s="27">
         <v>1.9463441675685741E-2</v>
       </c>
-      <c r="P29" s="44">
+      <c r="P29" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q29" s="42">
+      <c r="Q29" s="41">
         <v>5.8975999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="39">
+      <c r="A30" s="55">
         <v>45413</v>
       </c>
-      <c r="B30" s="40">
+      <c r="B30" s="39">
         <v>113</v>
       </c>
-      <c r="C30" s="40">
+      <c r="C30" s="39">
         <v>161.99999999999997</v>
       </c>
-      <c r="D30" s="40">
+      <c r="D30" s="39">
         <v>2</v>
       </c>
       <c r="E30">
@@ -4775,7 +4763,7 @@
         <f t="shared" si="3"/>
         <v>0.11793327569169319</v>
       </c>
-      <c r="H30" s="52">
+      <c r="H30" s="51">
         <f t="shared" si="4"/>
         <v>97.356092071467756</v>
       </c>
@@ -4783,15 +4771,15 @@
         <f t="shared" si="2"/>
         <v>45.2</v>
       </c>
-      <c r="J30" s="47">
+      <c r="J30" s="46">
         <f t="shared" si="5"/>
         <v>266.88567723369965</v>
       </c>
-      <c r="K30" s="47">
+      <c r="K30" s="46">
         <f t="shared" si="6"/>
         <v>88.412471999999994</v>
       </c>
-      <c r="L30" s="47">
+      <c r="L30" s="46">
         <f t="shared" si="7"/>
         <v>178.47320523369967</v>
       </c>
@@ -4804,24 +4792,24 @@
       <c r="O30" s="27">
         <v>2.83426929938656E-2</v>
       </c>
-      <c r="P30" s="44">
+      <c r="P30" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q30" s="42">
+      <c r="Q30" s="41">
         <v>5.9045503812765405</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="39">
+      <c r="A31" s="55">
         <v>45444</v>
       </c>
-      <c r="B31" s="40">
-        <v>0</v>
-      </c>
-      <c r="C31" s="40">
-        <v>0</v>
-      </c>
-      <c r="D31" s="40">
+      <c r="B31" s="39">
+        <v>0</v>
+      </c>
+      <c r="C31" s="39">
+        <v>0</v>
+      </c>
+      <c r="D31" s="39">
         <v>0</v>
       </c>
       <c r="E31">
@@ -4836,7 +4824,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H31" s="52" t="e">
+      <c r="H31" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4844,15 +4832,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J31" s="47">
+      <c r="J31" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K31" s="47">
+      <c r="K31" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L31" s="47">
+      <c r="L31" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4865,24 +4853,24 @@
       <c r="O31" s="27">
         <v>3.6478268557543055E-2</v>
       </c>
-      <c r="P31" s="44">
+      <c r="P31" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q31" s="42">
+      <c r="Q31" s="41">
         <v>5.9391037362319556</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="39">
+      <c r="A32" s="55">
         <v>45474</v>
       </c>
-      <c r="B32" s="40">
+      <c r="B32" s="39">
         <v>668</v>
       </c>
-      <c r="C32" s="40">
+      <c r="C32" s="39">
         <v>994.68</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="39">
         <v>5</v>
       </c>
       <c r="E32">
@@ -4897,7 +4885,7 @@
         <f t="shared" si="3"/>
         <v>0.67797625917021065</v>
       </c>
-      <c r="H32" s="52">
+      <c r="H32" s="51">
         <f t="shared" si="4"/>
         <v>94.67672758543695</v>
       </c>
@@ -4905,15 +4893,15 @@
         <f t="shared" si="2"/>
         <v>267.2</v>
       </c>
-      <c r="J32" s="47">
+      <c r="J32" s="46">
         <f t="shared" si="5"/>
         <v>1585.9033876765286</v>
       </c>
-      <c r="K32" s="47">
+      <c r="K32" s="46">
         <f t="shared" si="6"/>
         <v>558.06919272000005</v>
       </c>
-      <c r="L32" s="47">
+      <c r="L32" s="46">
         <f t="shared" si="7"/>
         <v>1027.8341949565286</v>
       </c>
@@ -4926,24 +4914,24 @@
       <c r="O32" s="27">
         <v>5.7065480284115871E-2</v>
       </c>
-      <c r="P32" s="44">
+      <c r="P32" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q32" s="42">
+      <c r="Q32" s="41">
         <v>5.9352671694480863</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="39">
+      <c r="A33" s="55">
         <v>45505</v>
       </c>
-      <c r="B33" s="40">
-        <v>0</v>
-      </c>
-      <c r="C33" s="40">
-        <v>0</v>
-      </c>
-      <c r="D33" s="40">
+      <c r="B33" s="39">
+        <v>0</v>
+      </c>
+      <c r="C33" s="39">
+        <v>0</v>
+      </c>
+      <c r="D33" s="39">
         <v>0</v>
       </c>
       <c r="E33">
@@ -4958,7 +4946,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H33" s="52" t="e">
+      <c r="H33" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -4966,15 +4954,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J33" s="47">
+      <c r="J33" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K33" s="47">
+      <c r="K33" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L33" s="47">
+      <c r="L33" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4987,24 +4975,24 @@
       <c r="O33" s="27">
         <v>7.3904145474031777E-2</v>
       </c>
-      <c r="P33" s="44">
+      <c r="P33" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q33" s="42">
+      <c r="Q33" s="41">
         <v>5.9554631704407912</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="39">
+      <c r="A34" s="55">
         <v>45536</v>
       </c>
-      <c r="B34" s="40">
-        <v>0</v>
-      </c>
-      <c r="C34" s="40">
-        <v>0</v>
-      </c>
-      <c r="D34" s="40">
+      <c r="B34" s="39">
+        <v>0</v>
+      </c>
+      <c r="C34" s="39">
+        <v>0</v>
+      </c>
+      <c r="D34" s="39">
         <v>0</v>
       </c>
       <c r="E34">
@@ -5019,7 +5007,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H34" s="52" t="e">
+      <c r="H34" s="51" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -5027,15 +5015,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J34" s="47">
+      <c r="J34" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K34" s="47">
+      <c r="K34" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L34" s="47">
+      <c r="L34" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5048,24 +5036,24 @@
       <c r="O34" s="27">
         <v>9.1656076504074896E-2</v>
       </c>
-      <c r="P34" s="44">
+      <c r="P34" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q34" s="42">
+      <c r="Q34" s="41">
         <v>5.9398075895241602</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="39">
+      <c r="A35" s="55">
         <v>45566</v>
       </c>
-      <c r="B35" s="40">
+      <c r="B35" s="39">
         <v>104</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="39">
         <v>145.80000000000001</v>
       </c>
-      <c r="D35" s="40">
+      <c r="D35" s="39">
         <v>1</v>
       </c>
       <c r="E35">
@@ -5080,7 +5068,7 @@
         <f t="shared" si="3"/>
         <v>9.9764325782687902E-2</v>
       </c>
-      <c r="H35" s="52">
+      <c r="H35" s="51">
         <f t="shared" si="4"/>
         <v>89.48436224767498</v>
       </c>
@@ -5088,15 +5076,15 @@
         <f t="shared" si="2"/>
         <v>41.6</v>
       </c>
-      <c r="J35" s="47">
+      <c r="J35" s="46">
         <f t="shared" si="5"/>
         <v>251.23115011307976</v>
       </c>
-      <c r="K35" s="47">
+      <c r="K35" s="46">
         <f t="shared" si="6"/>
         <v>75.466517400000015</v>
       </c>
-      <c r="L35" s="47">
+      <c r="L35" s="46">
         <f t="shared" si="7"/>
         <v>175.76463271307975</v>
       </c>
@@ -5109,24 +5097,24 @@
       <c r="O35" s="27">
         <v>0.11272763670492415</v>
       </c>
-      <c r="P35" s="44">
+      <c r="P35" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q35" s="42">
+      <c r="Q35" s="41">
         <v>6.0392103392567247</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="39">
+      <c r="A36" s="55">
         <v>45597</v>
       </c>
-      <c r="B36" s="40">
+      <c r="B36" s="39">
         <v>194</v>
       </c>
-      <c r="C36" s="40">
+      <c r="C36" s="39">
         <v>324</v>
       </c>
-      <c r="D36" s="40">
+      <c r="D36" s="39">
         <v>3</v>
       </c>
       <c r="E36">
@@ -5141,7 +5129,7 @@
         <f t="shared" si="3"/>
         <v>0.19437294532805505</v>
       </c>
-      <c r="H36" s="52">
+      <c r="H36" s="51">
         <f t="shared" si="4"/>
         <v>93.462910316998318</v>
       </c>
@@ -5149,15 +5137,15 @@
         <f t="shared" si="2"/>
         <v>77.599999999999994</v>
       </c>
-      <c r="J36" s="47">
+      <c r="J36" s="46">
         <f t="shared" si="5"/>
         <v>468.6427223263218</v>
       </c>
-      <c r="K36" s="47">
+      <c r="K36" s="46">
         <f t="shared" si="6"/>
         <v>167.49665999999999</v>
       </c>
-      <c r="L36" s="47">
+      <c r="L36" s="46">
         <f t="shared" si="7"/>
         <v>301.14606232632184</v>
       </c>
@@ -5170,24 +5158,24 @@
       <c r="O36" s="27">
         <v>7.0077601401778142E-2</v>
       </c>
-      <c r="P36" s="44">
+      <c r="P36" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q36" s="42">
+      <c r="Q36" s="41">
         <v>6.0392103392567247</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="39">
+      <c r="A37" s="55">
         <v>45627</v>
       </c>
-      <c r="B37" s="40">
+      <c r="B37" s="39">
         <v>74</v>
       </c>
-      <c r="C37" s="40">
+      <c r="C37" s="39">
         <v>93.96</v>
       </c>
-      <c r="D37" s="40">
+      <c r="D37" s="39">
         <v>1</v>
       </c>
       <c r="E37">
@@ -5202,7 +5190,7 @@
         <f t="shared" si="3"/>
         <v>7.5156860177017393E-2</v>
       </c>
-      <c r="H37" s="52">
+      <c r="H37" s="51">
         <f t="shared" si="4"/>
         <v>94.741907242105427</v>
       </c>
@@ -5210,15 +5198,15 @@
         <f t="shared" si="2"/>
         <v>29.6</v>
       </c>
-      <c r="J37" s="47">
+      <c r="J37" s="46">
         <f t="shared" si="5"/>
         <v>178.76062604199905</v>
       </c>
-      <c r="K37" s="47">
+      <c r="K37" s="46">
         <f t="shared" si="6"/>
         <v>48.859575839999998</v>
       </c>
-      <c r="L37" s="47">
+      <c r="L37" s="46">
         <f t="shared" si="7"/>
         <v>129.90105020199906</v>
       </c>
@@ -5231,10 +5219,10 @@
       <c r="O37" s="27">
         <v>5.6366754364629776E-2</v>
       </c>
-      <c r="P37" s="44">
+      <c r="P37" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q37" s="42">
+      <c r="Q37" s="41">
         <v>6.0392103392567247</v>
       </c>
     </row>
@@ -5257,12 +5245,12 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H37"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -5279,60 +5267,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="C1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="E1" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="42" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="39">
+      <c r="A2" s="55">
         <v>44562</v>
       </c>
       <c r="B2" s="31">
@@ -5356,7 +5344,7 @@
         <f>(E2-F2)/1000</f>
         <v>0</v>
       </c>
-      <c r="H2" s="46" t="e">
+      <c r="H2" s="45" t="e">
         <f t="shared" ref="H2:H3" si="2">(E2-F2)/E2</f>
         <v>#DIV/0!</v>
       </c>
@@ -5364,15 +5352,15 @@
         <f t="shared" ref="I2:I37" si="3">B2/P2</f>
         <v>0</v>
       </c>
-      <c r="J2" s="47">
+      <c r="J2" s="46">
         <f>I2*Q2</f>
         <v>0</v>
       </c>
-      <c r="K2" s="47">
+      <c r="K2" s="46">
         <f>C2*M2</f>
         <v>0</v>
       </c>
-      <c r="L2" s="47">
+      <c r="L2" s="46">
         <f>J2-K2</f>
         <v>0</v>
       </c>
@@ -5385,15 +5373,15 @@
       <c r="O2" s="27">
         <v>7.3200000000000001E-2</v>
       </c>
-      <c r="P2" s="44">
+      <c r="P2" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q2" s="42">
+      <c r="Q2" s="41">
         <v>5.49</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="39">
+      <c r="A3" s="55">
         <v>44593</v>
       </c>
       <c r="B3" s="31">
@@ -5417,7 +5405,7 @@
         <f t="shared" ref="G3:G37" si="4">(E3-F3)/1000</f>
         <v>0</v>
       </c>
-      <c r="H3" s="46" t="e">
+      <c r="H3" s="45" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -5425,15 +5413,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J3" s="47">
+      <c r="J3" s="46">
         <f t="shared" ref="J3:J37" si="5">I3*Q3</f>
         <v>0</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="46">
         <f t="shared" ref="K3:K37" si="6">C3*M3</f>
         <v>0</v>
       </c>
-      <c r="L3" s="47">
+      <c r="L3" s="46">
         <f t="shared" ref="L3:L37" si="7">J3-K3</f>
         <v>0</v>
       </c>
@@ -5446,15 +5434,15 @@
       <c r="O3" s="27">
         <v>5.0254040888372771E-2</v>
       </c>
-      <c r="P3" s="44">
+      <c r="P3" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q3" s="42">
+      <c r="Q3" s="41">
         <v>5.6</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="39">
+      <c r="A4" s="55">
         <v>44621</v>
       </c>
       <c r="B4" s="31">
@@ -5463,7 +5451,7 @@
       <c r="C4" s="31">
         <v>440.64</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="47">
         <v>2</v>
       </c>
       <c r="E4">
@@ -5478,7 +5466,7 @@
         <f t="shared" si="4"/>
         <v>0.25807311835780716</v>
       </c>
-      <c r="H4" s="51">
+      <c r="H4" s="50">
         <f>((E4-F4)/E4)*100</f>
         <v>96.211273764835894</v>
       </c>
@@ -5486,15 +5474,15 @@
         <f t="shared" si="3"/>
         <v>100.08799999999999</v>
       </c>
-      <c r="J4" s="47">
+      <c r="J4" s="46">
         <f t="shared" si="5"/>
         <v>627.55175999999994</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="46">
         <f t="shared" si="6"/>
         <v>176.6591856</v>
       </c>
-      <c r="L4" s="47">
+      <c r="L4" s="46">
         <f t="shared" si="7"/>
         <v>450.89257439999994</v>
       </c>
@@ -5507,15 +5495,15 @@
       <c r="O4" s="27">
         <v>4.0615145240959265E-2</v>
       </c>
-      <c r="P4" s="44">
+      <c r="P4" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q4" s="42">
+      <c r="Q4" s="41">
         <v>6.27</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="39">
+      <c r="A5" s="55">
         <v>44652</v>
       </c>
       <c r="B5" s="31">
@@ -5524,7 +5512,7 @@
       <c r="C5" s="31">
         <v>1172.8800000000001</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="47">
         <v>5</v>
       </c>
       <c r="E5">
@@ -5539,7 +5527,7 @@
         <f t="shared" si="4"/>
         <v>0.68113956728695613</v>
       </c>
-      <c r="H5" s="51">
+      <c r="H5" s="50">
         <f t="shared" ref="H5:H37" si="8">((E5-F5)/E5)*100</f>
         <v>97.986180491101635</v>
       </c>
@@ -5547,15 +5535,15 @@
         <f t="shared" si="3"/>
         <v>259.38</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="46">
         <f t="shared" si="5"/>
         <v>1714.5018</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="46">
         <f t="shared" si="6"/>
         <v>479.06987328000002</v>
       </c>
-      <c r="L5" s="47">
+      <c r="L5" s="46">
         <f t="shared" si="7"/>
         <v>1235.4319267199999</v>
       </c>
@@ -5568,15 +5556,15 @@
       <c r="O5" s="27">
         <v>2.1588145135390389E-2</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q5" s="42">
+      <c r="Q5" s="41">
         <v>6.61</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
+      <c r="A6" s="55">
         <v>44682</v>
       </c>
       <c r="B6" s="31">
@@ -5585,7 +5573,7 @@
       <c r="C6" s="31">
         <v>3204.36</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="47">
         <v>15</v>
       </c>
       <c r="E6">
@@ -5600,7 +5588,7 @@
         <f t="shared" si="4"/>
         <v>2.1297085351321119</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="50">
         <f t="shared" si="8"/>
         <v>97.385706354811958</v>
       </c>
@@ -5608,15 +5596,15 @@
         <f t="shared" si="3"/>
         <v>816</v>
       </c>
-      <c r="J6" s="47">
+      <c r="J6" s="46">
         <f t="shared" si="5"/>
         <v>5597.76</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="46">
         <f t="shared" si="6"/>
         <v>1328.14633716</v>
       </c>
-      <c r="L6" s="47">
+      <c r="L6" s="46">
         <f t="shared" si="7"/>
         <v>4269.61366284</v>
       </c>
@@ -5629,15 +5617,15 @@
       <c r="O6" s="27">
         <v>2.8025227876415777E-2</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q6" s="42">
+      <c r="Q6" s="41">
         <v>6.86</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
+      <c r="A7" s="55">
         <v>44713</v>
       </c>
       <c r="B7" s="31">
@@ -5646,7 +5634,7 @@
       <c r="C7" s="31">
         <v>849</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="47">
         <v>4</v>
       </c>
       <c r="E7">
@@ -5661,7 +5649,7 @@
         <f t="shared" si="4"/>
         <v>0.55457330359691459</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="50">
         <f t="shared" si="8"/>
         <v>95.889868935601399</v>
       </c>
@@ -5669,15 +5657,15 @@
         <f t="shared" si="3"/>
         <v>215.8</v>
       </c>
-      <c r="J7" s="47">
+      <c r="J7" s="46">
         <f t="shared" si="5"/>
         <v>1553.7600000000002</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="46">
         <f t="shared" si="6"/>
         <v>347.74530600000003</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="46">
         <f t="shared" si="7"/>
         <v>1206.0146940000002</v>
       </c>
@@ -5690,15 +5678,15 @@
       <c r="O7" s="27">
         <v>4.4060605010353047E-2</v>
       </c>
-      <c r="P7" s="44">
+      <c r="P7" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q7" s="42">
+      <c r="Q7" s="41">
         <v>7.2</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="39">
+      <c r="A8" s="55">
         <v>44743</v>
       </c>
       <c r="B8" s="31">
@@ -5707,7 +5695,7 @@
       <c r="C8" s="31">
         <v>3622.32</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="47">
         <v>18</v>
       </c>
       <c r="E8">
@@ -5722,7 +5710,7 @@
         <f t="shared" si="4"/>
         <v>2.5697420523901062</v>
       </c>
-      <c r="H8" s="51">
+      <c r="H8" s="50">
         <f t="shared" si="8"/>
         <v>96.094614980981447</v>
       </c>
@@ -5730,15 +5718,15 @@
         <f t="shared" si="3"/>
         <v>997.82800000000009</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="46">
         <f t="shared" si="5"/>
         <v>7413.86204</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="46">
         <f t="shared" si="6"/>
         <v>1361.7025343999999</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="46">
         <f t="shared" si="7"/>
         <v>6052.1595056000006</v>
       </c>
@@ -5751,15 +5739,15 @@
       <c r="O8" s="27">
         <v>4.1865727403878748E-2</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q8" s="42">
+      <c r="Q8" s="41">
         <v>7.43</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
+      <c r="A9" s="55">
         <v>44774</v>
       </c>
       <c r="B9" s="31">
@@ -5768,7 +5756,7 @@
       <c r="C9" s="31">
         <v>4390.2</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="47">
         <v>18</v>
       </c>
       <c r="E9">
@@ -5783,7 +5771,7 @@
         <f t="shared" si="4"/>
         <v>3.3321861834141582</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="50">
         <f t="shared" si="8"/>
         <v>95.735627064526227</v>
       </c>
@@ -5791,15 +5779,15 @@
         <f t="shared" si="3"/>
         <v>1298.7360000000001</v>
       </c>
-      <c r="J9" s="47">
+      <c r="J9" s="46">
         <f t="shared" si="5"/>
         <v>9208.0382399999999</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="46">
         <f t="shared" si="6"/>
         <v>1812.0594401999999</v>
       </c>
-      <c r="L9" s="47">
+      <c r="L9" s="46">
         <f t="shared" si="7"/>
         <v>7395.9787998000002</v>
       </c>
@@ -5812,15 +5800,15 @@
       <c r="O9" s="27">
         <v>4.5714077868278892E-2</v>
       </c>
-      <c r="P9" s="44">
+      <c r="P9" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q9" s="42">
+      <c r="Q9" s="41">
         <v>7.09</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
+      <c r="A10" s="55">
         <v>44805</v>
       </c>
       <c r="B10" s="31">
@@ -5844,7 +5832,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H10" s="51" t="e">
+      <c r="H10" s="50" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -5852,15 +5840,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J10" s="47">
+      <c r="J10" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K10" s="47">
+      <c r="K10" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5873,15 +5861,15 @@
       <c r="O10" s="27">
         <v>4.9086599685372614E-2</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q10" s="42">
+      <c r="Q10" s="41">
         <v>6.84</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="A11" s="55">
         <v>44835</v>
       </c>
       <c r="B11" s="31">
@@ -5890,7 +5878,7 @@
       <c r="C11" s="31">
         <v>3285.36</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="47">
         <v>16</v>
       </c>
       <c r="E11">
@@ -5905,7 +5893,7 @@
         <f t="shared" si="4"/>
         <v>2.2398435520219429</v>
       </c>
-      <c r="H11" s="51">
+      <c r="H11" s="50">
         <f t="shared" si="8"/>
         <v>95.603999969248463</v>
       </c>
@@ -5913,15 +5901,15 @@
         <f t="shared" si="3"/>
         <v>874.19200000000001</v>
       </c>
-      <c r="J11" s="47">
+      <c r="J11" s="46">
         <f t="shared" si="5"/>
         <v>5656.0222400000002</v>
       </c>
-      <c r="K11" s="47">
+      <c r="K11" s="46">
         <f t="shared" si="6"/>
         <v>1358.8051838400002</v>
       </c>
-      <c r="L11" s="47">
+      <c r="L11" s="46">
         <f t="shared" si="7"/>
         <v>4297.2170561599996</v>
       </c>
@@ -5934,15 +5922,15 @@
       <c r="O11" s="27">
         <v>4.7125120329656413E-2</v>
       </c>
-      <c r="P11" s="44">
+      <c r="P11" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q11" s="42">
+      <c r="Q11" s="41">
         <v>6.47</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="A12" s="55">
         <v>44866</v>
       </c>
       <c r="B12" s="31">
@@ -5951,7 +5939,7 @@
       <c r="C12" s="31">
         <v>4205.5200000000004</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="47">
         <v>18</v>
       </c>
       <c r="E12">
@@ -5966,7 +5954,7 @@
         <f t="shared" si="4"/>
         <v>2.5978289685407532</v>
       </c>
-      <c r="H12" s="51">
+      <c r="H12" s="50">
         <f t="shared" si="8"/>
         <v>96.245950681126573</v>
       </c>
@@ -5974,15 +5962,15 @@
         <f t="shared" si="3"/>
         <v>1007.1479999999999</v>
       </c>
-      <c r="J12" s="47">
+      <c r="J12" s="46">
         <f t="shared" si="5"/>
         <v>6546.4619999999995</v>
       </c>
-      <c r="K12" s="47">
+      <c r="K12" s="46">
         <f t="shared" si="6"/>
         <v>1728.98179344</v>
       </c>
-      <c r="L12" s="47">
+      <c r="L12" s="46">
         <f t="shared" si="7"/>
         <v>4817.4802065599997</v>
       </c>
@@ -5995,15 +5983,15 @@
       <c r="O12" s="27">
         <v>4.0243408698322984E-2</v>
       </c>
-      <c r="P12" s="44">
+      <c r="P12" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q12" s="42">
+      <c r="Q12" s="41">
         <v>6.5</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="39">
+      <c r="A13" s="55">
         <v>44896</v>
       </c>
       <c r="B13" s="31">
@@ -6012,7 +6000,7 @@
       <c r="C13" s="31">
         <v>1166.4000000000001</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="47">
         <v>5</v>
       </c>
       <c r="E13">
@@ -6027,7 +6015,7 @@
         <f t="shared" si="4"/>
         <v>0.74314603916005217</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H13" s="50">
         <f t="shared" si="8"/>
         <v>97.260402587844894</v>
       </c>
@@ -6035,15 +6023,15 @@
         <f t="shared" si="3"/>
         <v>285.10399999999998</v>
       </c>
-      <c r="J13" s="47">
+      <c r="J13" s="46">
         <f t="shared" si="5"/>
         <v>1810.4103999999998</v>
       </c>
-      <c r="K13" s="47">
+      <c r="K13" s="46">
         <f t="shared" si="6"/>
         <v>487.1049696</v>
       </c>
-      <c r="L13" s="47">
+      <c r="L13" s="46">
         <f t="shared" si="7"/>
         <v>1323.3054303999998</v>
       </c>
@@ -6056,15 +6044,15 @@
       <c r="O13" s="27">
         <v>2.9368484258302584E-2</v>
       </c>
-      <c r="P13" s="44">
+      <c r="P13" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q13" s="42">
+      <c r="Q13" s="41">
         <v>6.35</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="A14" s="55">
         <v>44927</v>
       </c>
       <c r="B14" s="31">
@@ -6088,7 +6076,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H14" s="51" t="e">
+      <c r="H14" s="50" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -6096,15 +6084,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J14" s="47">
+      <c r="J14" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K14" s="47">
+      <c r="K14" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L14" s="47">
+      <c r="L14" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -6117,15 +6105,15 @@
       <c r="O14" s="27">
         <v>2.9173607327091757E-2</v>
       </c>
-      <c r="P14" s="44">
+      <c r="P14" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q14" s="42">
+      <c r="Q14" s="41">
         <v>6.3</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="39">
+      <c r="A15" s="55">
         <v>44958</v>
       </c>
       <c r="B15" s="31">
@@ -6149,7 +6137,7 @@
         <f t="shared" si="4"/>
         <v>3.6818946176375052E-2</v>
       </c>
-      <c r="H15" s="51">
+      <c r="H15" s="50">
         <f t="shared" si="8"/>
         <v>97.782297169954674</v>
       </c>
@@ -6157,15 +6145,15 @@
         <f t="shared" si="3"/>
         <v>14.05000000000012</v>
       </c>
-      <c r="J15" s="47">
+      <c r="J15" s="46">
         <f t="shared" si="5"/>
         <v>85.143000000000725</v>
       </c>
-      <c r="K15" s="47">
+      <c r="K15" s="46">
         <f t="shared" si="6"/>
         <v>20.671426799999999</v>
       </c>
-      <c r="L15" s="47">
+      <c r="L15" s="46">
         <f t="shared" si="7"/>
         <v>64.471573200000734</v>
       </c>
@@ -6178,15 +6166,15 @@
       <c r="O15" s="27">
         <v>2.3773774338085845E-2</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q15" s="42">
+      <c r="Q15" s="41">
         <v>6.06</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="39">
+      <c r="A16" s="55">
         <v>44986</v>
       </c>
       <c r="B16" s="31">
@@ -6210,7 +6198,7 @@
         <f t="shared" si="4"/>
         <v>3.124675014844628E-2</v>
       </c>
-      <c r="H16" s="51">
+      <c r="H16" s="50">
         <f t="shared" si="8"/>
         <v>97.24132718946197</v>
       </c>
@@ -6218,15 +6206,15 @@
         <f t="shared" si="3"/>
         <v>11.9900000000008</v>
       </c>
-      <c r="J16" s="47">
+      <c r="J16" s="46">
         <f t="shared" si="5"/>
         <v>70.3813000000047</v>
       </c>
-      <c r="K16" s="47">
+      <c r="K16" s="46">
         <f t="shared" si="6"/>
         <v>19.397795760000001</v>
       </c>
-      <c r="L16" s="47">
+      <c r="L16" s="46">
         <f t="shared" si="7"/>
         <v>50.983504240004699</v>
       </c>
@@ -6239,15 +6227,15 @@
       <c r="O16" s="27">
         <v>2.9572972528967699E-2</v>
       </c>
-      <c r="P16" s="44">
+      <c r="P16" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q16" s="42">
+      <c r="Q16" s="41">
         <v>5.87</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="39">
+      <c r="A17" s="55">
         <v>45017</v>
       </c>
       <c r="B17" s="31">
@@ -6271,7 +6259,7 @@
         <f t="shared" si="4"/>
         <v>2.348933456460604E-2</v>
       </c>
-      <c r="H17" s="51">
+      <c r="H17" s="50">
         <f t="shared" si="8"/>
         <v>96.825862531448294</v>
       </c>
@@ -6279,15 +6267,15 @@
         <f t="shared" si="3"/>
         <v>9.0519999999987988</v>
       </c>
-      <c r="J17" s="47">
+      <c r="J17" s="46">
         <f t="shared" si="5"/>
         <v>51.958479999993109</v>
       </c>
-      <c r="K17" s="47">
+      <c r="K17" s="46">
         <f t="shared" si="6"/>
         <v>28.423778040000002</v>
       </c>
-      <c r="L17" s="47">
+      <c r="L17" s="46">
         <f t="shared" si="7"/>
         <v>23.534701959993107</v>
       </c>
@@ -6300,15 +6288,15 @@
       <c r="O17" s="27">
         <v>3.40267536628742E-2</v>
       </c>
-      <c r="P17" s="44">
+      <c r="P17" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q17" s="42">
+      <c r="Q17" s="41">
         <v>5.74</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
+      <c r="A18" s="55">
         <v>45047</v>
       </c>
       <c r="B18" s="31">
@@ -6332,7 +6320,7 @@
         <f t="shared" si="4"/>
         <v>0.11413171946824212</v>
       </c>
-      <c r="H18" s="51">
+      <c r="H18" s="50">
         <f t="shared" si="8"/>
         <v>97.247128443891285</v>
       </c>
@@ -6340,15 +6328,15 @@
         <f t="shared" si="3"/>
         <v>43.79200000000121</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="46">
         <f t="shared" si="5"/>
         <v>235.60096000000649</v>
       </c>
-      <c r="K18" s="47">
+      <c r="K18" s="46">
         <f t="shared" si="6"/>
         <v>72.225775439999992</v>
       </c>
-      <c r="L18" s="47">
+      <c r="L18" s="46">
         <f t="shared" si="7"/>
         <v>163.37518456000652</v>
       </c>
@@ -6361,15 +6349,15 @@
       <c r="O18" s="27">
         <v>2.9510783081485501E-2</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q18" s="42">
+      <c r="Q18" s="41">
         <v>5.38</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="39">
+      <c r="A19" s="55">
         <v>45078</v>
       </c>
       <c r="B19" s="31">
@@ -6393,7 +6381,7 @@
         <f t="shared" si="4"/>
         <v>3.5621466265109578E-2</v>
       </c>
-      <c r="H19" s="51">
+      <c r="H19" s="50">
         <f t="shared" si="8"/>
         <v>95.075764592033323</v>
       </c>
@@ -6401,15 +6389,15 @@
         <f t="shared" si="3"/>
         <v>13.98</v>
       </c>
-      <c r="J19" s="47">
+      <c r="J19" s="46">
         <f t="shared" si="5"/>
         <v>70.599000000000004</v>
       </c>
-      <c r="K19" s="47">
+      <c r="K19" s="46">
         <f t="shared" si="6"/>
         <v>22.13469504</v>
       </c>
-      <c r="L19" s="47">
+      <c r="L19" s="46">
         <f t="shared" si="7"/>
         <v>48.464304960000007</v>
       </c>
@@ -6422,15 +6410,15 @@
       <c r="O19" s="27">
         <v>5.2787803573402799E-2</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q19" s="42">
+      <c r="Q19" s="41">
         <v>5.05</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="39">
+      <c r="A20" s="55">
         <v>45108</v>
       </c>
       <c r="B20" s="31">
@@ -6454,7 +6442,7 @@
         <f t="shared" si="4"/>
         <v>2.8435446617381812E-2</v>
       </c>
-      <c r="H20" s="51">
+      <c r="H20" s="50">
         <f t="shared" si="8"/>
         <v>95.38152890275154</v>
       </c>
@@ -6462,15 +6450,15 @@
         <f t="shared" si="3"/>
         <v>11.124000000000402</v>
       </c>
-      <c r="J20" s="47">
+      <c r="J20" s="46">
         <f t="shared" si="5"/>
         <v>55.620000000002008</v>
       </c>
-      <c r="K20" s="47">
+      <c r="K20" s="46">
         <f t="shared" si="6"/>
         <v>18.29490624</v>
       </c>
-      <c r="L20" s="47">
+      <c r="L20" s="46">
         <f t="shared" si="7"/>
         <v>37.325093760002005</v>
       </c>
@@ -6483,15 +6471,15 @@
       <c r="O20" s="27">
         <v>4.9510010162503372E-2</v>
       </c>
-      <c r="P20" s="44">
+      <c r="P20" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q20" s="42">
+      <c r="Q20" s="41">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
+      <c r="A21" s="55">
         <v>45139</v>
       </c>
       <c r="B21" s="31">
@@ -6515,7 +6503,7 @@
         <f t="shared" si="4"/>
         <v>0.52226026039065609</v>
       </c>
-      <c r="H21" s="51">
+      <c r="H21" s="50">
         <f t="shared" si="8"/>
         <v>96.091337026159152</v>
       </c>
@@ -6523,15 +6511,15 @@
         <f t="shared" si="3"/>
         <v>202.8</v>
       </c>
-      <c r="J21" s="47">
+      <c r="J21" s="46">
         <f t="shared" si="5"/>
         <v>1121.4840000000002</v>
       </c>
-      <c r="K21" s="47">
+      <c r="K21" s="46">
         <f t="shared" si="6"/>
         <v>391.77205199999997</v>
       </c>
-      <c r="L21" s="47">
+      <c r="L21" s="46">
         <f t="shared" si="7"/>
         <v>729.71194800000012</v>
       </c>
@@ -6544,15 +6532,15 @@
       <c r="O21" s="27">
         <v>4.1900867079573897E-2</v>
       </c>
-      <c r="P21" s="44">
+      <c r="P21" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q21" s="42">
+      <c r="Q21" s="41">
         <v>5.53</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="A22" s="55">
         <v>45170</v>
       </c>
       <c r="B22" s="31">
@@ -6576,7 +6564,7 @@
         <f t="shared" si="4"/>
         <v>0.62986297313298101</v>
       </c>
-      <c r="H22" s="51">
+      <c r="H22" s="50">
         <f t="shared" si="8"/>
         <v>96.797157099538495</v>
       </c>
@@ -6584,15 +6572,15 @@
         <f t="shared" si="3"/>
         <v>242.8</v>
       </c>
-      <c r="J22" s="47">
+      <c r="J22" s="46">
         <f t="shared" si="5"/>
         <v>1473.796</v>
       </c>
-      <c r="K22" s="47">
+      <c r="K22" s="46">
         <f t="shared" si="6"/>
         <v>599.00235803999999</v>
       </c>
-      <c r="L22" s="47">
+      <c r="L22" s="46">
         <f t="shared" si="7"/>
         <v>874.79364196000006</v>
       </c>
@@ -6605,15 +6593,15 @@
       <c r="O22" s="27">
         <v>3.4334475892947448E-2</v>
       </c>
-      <c r="P22" s="44">
+      <c r="P22" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q22" s="42">
+      <c r="Q22" s="41">
         <v>6.07</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
+      <c r="A23" s="55">
         <v>45200</v>
       </c>
       <c r="B23" s="31">
@@ -6637,7 +6625,7 @@
         <f t="shared" si="4"/>
         <v>1.7056297840641126</v>
       </c>
-      <c r="H23" s="51">
+      <c r="H23" s="50">
         <f t="shared" si="8"/>
         <v>96.387164296653935</v>
       </c>
@@ -6645,15 +6633,15 @@
         <f t="shared" si="3"/>
         <v>660.28400000000113</v>
       </c>
-      <c r="J23" s="47">
+      <c r="J23" s="46">
         <f t="shared" si="5"/>
         <v>4014.5267200000071</v>
       </c>
-      <c r="K23" s="47">
+      <c r="K23" s="46">
         <f t="shared" si="6"/>
         <v>1797.1066295999999</v>
       </c>
-      <c r="L23" s="47">
+      <c r="L23" s="46">
         <f t="shared" si="7"/>
         <v>2217.4200904000072</v>
       </c>
@@ -6666,15 +6654,15 @@
       <c r="O23" s="27">
         <v>3.8729598739869808E-2</v>
       </c>
-      <c r="P23" s="44">
+      <c r="P23" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q23" s="42">
+      <c r="Q23" s="41">
         <v>6.08</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="39">
+      <c r="A24" s="55">
         <v>45231</v>
       </c>
       <c r="B24" s="31">
@@ -6698,7 +6686,7 @@
         <f t="shared" si="4"/>
         <v>2.3489663251486261</v>
       </c>
-      <c r="H24" s="51">
+      <c r="H24" s="50">
         <f t="shared" si="8"/>
         <v>95.062903695269299</v>
       </c>
@@ -6706,15 +6694,15 @@
         <f t="shared" si="3"/>
         <v>922</v>
       </c>
-      <c r="J24" s="47">
+      <c r="J24" s="46">
         <f t="shared" si="5"/>
         <v>5605.76</v>
       </c>
-      <c r="K24" s="47">
+      <c r="K24" s="46">
         <f t="shared" si="6"/>
         <v>1904.8585190400001</v>
       </c>
-      <c r="L24" s="47">
+      <c r="L24" s="46">
         <f t="shared" si="7"/>
         <v>3700.9014809600003</v>
       </c>
@@ -6727,15 +6715,15 @@
       <c r="O24" s="27">
         <v>5.2925672386713071E-2</v>
       </c>
-      <c r="P24" s="44">
+      <c r="P24" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q24" s="42">
+      <c r="Q24" s="41">
         <v>6.08</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="39">
+      <c r="A25" s="55">
         <v>45261</v>
       </c>
       <c r="B25" s="31">
@@ -6759,7 +6747,7 @@
         <f t="shared" si="4"/>
         <v>0.56539847934350373</v>
       </c>
-      <c r="H25" s="51">
+      <c r="H25" s="50">
         <f t="shared" si="8"/>
         <v>95.721225882300786</v>
       </c>
@@ -6767,15 +6755,15 @@
         <f t="shared" si="3"/>
         <v>220.4</v>
       </c>
-      <c r="J25" s="47">
+      <c r="J25" s="46">
         <f t="shared" si="5"/>
         <v>1309.1760000000002</v>
       </c>
-      <c r="K25" s="47">
+      <c r="K25" s="46">
         <f t="shared" si="6"/>
         <v>464.82144191999998</v>
       </c>
-      <c r="L25" s="47">
+      <c r="L25" s="46">
         <f t="shared" si="7"/>
         <v>844.35455808000017</v>
       </c>
@@ -6788,15 +6776,15 @@
       <c r="O25" s="27">
         <v>4.586845854173565E-2</v>
       </c>
-      <c r="P25" s="44">
+      <c r="P25" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q25" s="42">
+      <c r="Q25" s="41">
         <v>5.94</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="39">
+      <c r="A26" s="55">
         <v>45292</v>
       </c>
       <c r="B26" s="32">
@@ -6820,7 +6808,7 @@
         <f t="shared" si="4"/>
         <v>2.9032876860325718</v>
       </c>
-      <c r="H26" s="51">
+      <c r="H26" s="50">
         <f t="shared" si="8"/>
         <v>96.072747495425887</v>
       </c>
@@ -6828,15 +6816,15 @@
         <f t="shared" si="3"/>
         <v>1127.5999999999999</v>
       </c>
-      <c r="J26" s="47">
+      <c r="J26" s="46">
         <f t="shared" si="5"/>
         <v>6630.2879999999996</v>
       </c>
-      <c r="K26" s="47">
+      <c r="K26" s="46">
         <f t="shared" si="6"/>
         <v>1803.3226214399997</v>
       </c>
-      <c r="L26" s="47">
+      <c r="L26" s="46">
         <f t="shared" si="7"/>
         <v>4826.9653785600003</v>
       </c>
@@ -6849,21 +6837,21 @@
       <c r="O26" s="27">
         <v>4.2100146849034403E-2</v>
       </c>
-      <c r="P26" s="44">
+      <c r="P26" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q26" s="42">
+      <c r="Q26" s="41">
         <v>5.88</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="39">
+      <c r="A27" s="55">
         <v>45323</v>
       </c>
       <c r="B27" s="33">
         <v>2748</v>
       </c>
-      <c r="C27" s="49">
+      <c r="C27" s="48">
         <v>2841.4800000000005</v>
       </c>
       <c r="D27" s="33">
@@ -6881,7 +6869,7 @@
         <f t="shared" si="4"/>
         <v>2.8425967340793821</v>
       </c>
-      <c r="H27" s="51">
+      <c r="H27" s="50">
         <f t="shared" si="8"/>
         <v>96.49476193267364</v>
       </c>
@@ -6889,15 +6877,15 @@
         <f t="shared" si="3"/>
         <v>1099.2</v>
       </c>
-      <c r="J27" s="47">
+      <c r="J27" s="46">
         <f t="shared" si="5"/>
         <v>6463.2960000000003</v>
       </c>
-      <c r="K27" s="47">
+      <c r="K27" s="46">
         <f t="shared" si="6"/>
         <v>1565.0502447600004</v>
       </c>
-      <c r="L27" s="47">
+      <c r="L27" s="46">
         <f t="shared" si="7"/>
         <v>4898.2457552400001</v>
       </c>
@@ -6910,15 +6898,15 @@
       <c r="O27" s="27">
         <v>3.7576152081738791E-2</v>
       </c>
-      <c r="P27" s="44">
+      <c r="P27" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q27" s="42">
+      <c r="Q27" s="41">
         <v>5.88</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="39">
+      <c r="A28" s="55">
         <v>45352</v>
       </c>
       <c r="B28" s="34">
@@ -6942,7 +6930,7 @@
         <f t="shared" si="4"/>
         <v>1.1026847294389805</v>
       </c>
-      <c r="H28" s="51">
+      <c r="H28" s="50">
         <f t="shared" si="8"/>
         <v>97.40755821734551</v>
       </c>
@@ -6950,15 +6938,15 @@
         <f t="shared" si="3"/>
         <v>422.4</v>
       </c>
-      <c r="J28" s="47">
+      <c r="J28" s="46">
         <f t="shared" si="5"/>
         <v>2193.6512407619584</v>
       </c>
-      <c r="K28" s="47">
+      <c r="K28" s="46">
         <f t="shared" si="6"/>
         <v>657.50506164000001</v>
       </c>
-      <c r="L28" s="47">
+      <c r="L28" s="46">
         <f t="shared" si="7"/>
         <v>1536.1461791219585</v>
       </c>
@@ -6971,15 +6959,15 @@
       <c r="O28" s="27">
         <v>2.7790975910056099E-2</v>
       </c>
-      <c r="P28" s="44">
+      <c r="P28" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q28" s="42">
+      <c r="Q28" s="41">
         <v>5.1933031268038796</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="39">
+      <c r="A29" s="55">
         <v>45383</v>
       </c>
       <c r="B29" s="34">
@@ -7003,7 +6991,7 @@
         <f t="shared" si="4"/>
         <v>0.93149485411701816</v>
       </c>
-      <c r="H29" s="51">
+      <c r="H29" s="50">
         <f t="shared" si="8"/>
         <v>98.184380440700963</v>
       </c>
@@ -7011,15 +6999,15 @@
         <f t="shared" si="3"/>
         <v>354</v>
       </c>
-      <c r="J29" s="47">
+      <c r="J29" s="46">
         <f t="shared" si="5"/>
         <v>2087.7503999999999</v>
       </c>
-      <c r="K29" s="47">
+      <c r="K29" s="46">
         <f t="shared" si="6"/>
         <v>615.31861247999996</v>
       </c>
-      <c r="L29" s="47">
+      <c r="L29" s="46">
         <f t="shared" si="7"/>
         <v>1472.4317875199999</v>
       </c>
@@ -7032,15 +7020,15 @@
       <c r="O29" s="27">
         <v>1.9463441675685741E-2</v>
       </c>
-      <c r="P29" s="44">
+      <c r="P29" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q29" s="42">
+      <c r="Q29" s="41">
         <v>5.8975999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="39">
+      <c r="A30" s="55">
         <v>45413</v>
       </c>
       <c r="B30" s="34">
@@ -7064,7 +7052,7 @@
         <f t="shared" si="4"/>
         <v>1.0499192508481712</v>
       </c>
-      <c r="H30" s="51">
+      <c r="H30" s="50">
         <f t="shared" si="8"/>
         <v>97.356092071467756</v>
       </c>
@@ -7072,15 +7060,15 @@
         <f t="shared" si="3"/>
         <v>402.4</v>
       </c>
-      <c r="J30" s="47">
+      <c r="J30" s="46">
         <f t="shared" si="5"/>
         <v>2375.9910734256796</v>
       </c>
-      <c r="K30" s="47">
+      <c r="K30" s="46">
         <f t="shared" si="6"/>
         <v>574.68106799999987</v>
       </c>
-      <c r="L30" s="47">
+      <c r="L30" s="46">
         <f t="shared" si="7"/>
         <v>1801.3100054256797</v>
       </c>
@@ -7093,15 +7081,15 @@
       <c r="O30" s="27">
         <v>2.83426929938656E-2</v>
       </c>
-      <c r="P30" s="44">
+      <c r="P30" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q30" s="42">
+      <c r="Q30" s="41">
         <v>5.9045503812765405</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="39">
+      <c r="A31" s="55">
         <v>45444</v>
       </c>
       <c r="B31" s="30">
@@ -7125,7 +7113,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H31" s="51" t="e">
+      <c r="H31" s="50" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -7133,15 +7121,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J31" s="47">
+      <c r="J31" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K31" s="47">
+      <c r="K31" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L31" s="47">
+      <c r="L31" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -7154,15 +7142,15 @@
       <c r="O31" s="27">
         <v>3.6478268557543055E-2</v>
       </c>
-      <c r="P31" s="44">
+      <c r="P31" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q31" s="42">
+      <c r="Q31" s="41">
         <v>5.9391037362319556</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="39">
+      <c r="A32" s="55">
         <v>45474</v>
       </c>
       <c r="B32" s="30">
@@ -7186,7 +7174,7 @@
         <f t="shared" si="4"/>
         <v>2.3739318416154531</v>
       </c>
-      <c r="H32" s="51">
+      <c r="H32" s="50">
         <f t="shared" si="8"/>
         <v>94.67672758543695</v>
       </c>
@@ -7194,15 +7182,15 @@
         <f t="shared" si="3"/>
         <v>935.6</v>
       </c>
-      <c r="J32" s="47">
+      <c r="J32" s="46">
         <f t="shared" si="5"/>
         <v>5553.0359637356296</v>
       </c>
-      <c r="K32" s="47">
+      <c r="K32" s="46">
         <f t="shared" si="6"/>
         <v>1594.2237199199999</v>
       </c>
-      <c r="L32" s="47">
+      <c r="L32" s="46">
         <f t="shared" si="7"/>
         <v>3958.8122438156297</v>
       </c>
@@ -7215,21 +7203,21 @@
       <c r="O32" s="27">
         <v>5.7065480284115871E-2</v>
       </c>
-      <c r="P32" s="44">
+      <c r="P32" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q32" s="42">
+      <c r="Q32" s="41">
         <v>5.9352671694480863</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="39">
+      <c r="A33" s="55">
         <v>45505</v>
       </c>
       <c r="B33" s="35">
         <v>525</v>
       </c>
-      <c r="C33" s="50">
+      <c r="C33" s="49">
         <v>680.4</v>
       </c>
       <c r="D33" s="35">
@@ -7247,7 +7235,7 @@
         <f t="shared" si="4"/>
         <v>0.52400032362613347</v>
       </c>
-      <c r="H33" s="51">
+      <c r="H33" s="50">
         <f t="shared" si="8"/>
         <v>93.105956578914956</v>
       </c>
@@ -7255,15 +7243,15 @@
         <f t="shared" si="3"/>
         <v>210</v>
       </c>
-      <c r="J33" s="47">
+      <c r="J33" s="46">
         <f t="shared" si="5"/>
         <v>1250.6472657925663</v>
       </c>
-      <c r="K33" s="47">
+      <c r="K33" s="46">
         <f t="shared" si="6"/>
         <v>354.29176440000003</v>
       </c>
-      <c r="L33" s="47">
+      <c r="L33" s="46">
         <f t="shared" si="7"/>
         <v>896.35550139256623</v>
       </c>
@@ -7276,15 +7264,15 @@
       <c r="O33" s="27">
         <v>7.3904145474031777E-2</v>
       </c>
-      <c r="P33" s="44">
+      <c r="P33" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q33" s="42">
+      <c r="Q33" s="41">
         <v>5.9554631704407912</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="39">
+      <c r="A34" s="55">
         <v>45536</v>
       </c>
       <c r="B34" s="35">
@@ -7308,7 +7296,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H34" s="51" t="e">
+      <c r="H34" s="50" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -7316,15 +7304,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J34" s="47">
+      <c r="J34" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K34" s="47">
+      <c r="K34" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L34" s="47">
+      <c r="L34" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -7337,21 +7325,21 @@
       <c r="O34" s="27">
         <v>9.1656076504074896E-2</v>
       </c>
-      <c r="P34" s="44">
+      <c r="P34" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q34" s="42">
+      <c r="Q34" s="41">
         <v>5.9398075895241602</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="39">
+      <c r="A35" s="55">
         <v>45566</v>
       </c>
       <c r="B35" s="35">
         <v>137</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C35" s="49">
         <v>343.44000000000005</v>
       </c>
       <c r="D35" s="35">
@@ -7369,7 +7357,7 @@
         <f t="shared" si="4"/>
         <v>0.13142031377142538</v>
       </c>
-      <c r="H35" s="51">
+      <c r="H35" s="50">
         <f t="shared" si="8"/>
         <v>89.48436224767498</v>
       </c>
@@ -7377,15 +7365,15 @@
         <f t="shared" si="3"/>
         <v>54.8</v>
       </c>
-      <c r="J35" s="47">
+      <c r="J35" s="46">
         <f t="shared" si="5"/>
         <v>330.9487265912685</v>
       </c>
-      <c r="K35" s="47">
+      <c r="K35" s="46">
         <f t="shared" si="6"/>
         <v>177.76557432000004</v>
       </c>
-      <c r="L35" s="47">
+      <c r="L35" s="46">
         <f t="shared" si="7"/>
         <v>153.18315227126845</v>
       </c>
@@ -7398,15 +7386,15 @@
       <c r="O35" s="27">
         <v>0.11272763670492415</v>
       </c>
-      <c r="P35" s="44">
+      <c r="P35" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q35" s="42">
+      <c r="Q35" s="41">
         <v>6.0392103392567247</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="39">
+      <c r="A36" s="55">
         <v>45597</v>
       </c>
       <c r="B36" s="35">
@@ -7430,7 +7418,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H36" s="51" t="e">
+      <c r="H36" s="50" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
@@ -7438,15 +7426,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J36" s="47">
+      <c r="J36" s="46">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K36" s="47">
+      <c r="K36" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L36" s="47">
+      <c r="L36" s="46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -7459,21 +7447,21 @@
       <c r="O36" s="27">
         <v>7.0077601401778142E-2</v>
       </c>
-      <c r="P36" s="44">
+      <c r="P36" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q36" s="42">
+      <c r="Q36" s="41">
         <v>6.0392103392567247</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="39">
+      <c r="A37" s="55">
         <v>45627</v>
       </c>
       <c r="B37" s="35">
         <v>41</v>
       </c>
-      <c r="C37" s="50">
+      <c r="C37" s="49">
         <v>100.44</v>
       </c>
       <c r="D37" s="35">
@@ -7491,7 +7479,7 @@
         <f t="shared" si="4"/>
         <v>4.1640963071050183E-2</v>
       </c>
-      <c r="H37" s="51">
+      <c r="H37" s="50">
         <f t="shared" si="8"/>
         <v>94.741907242105441</v>
       </c>
@@ -7499,15 +7487,15 @@
         <f t="shared" si="3"/>
         <v>16.399999999999999</v>
       </c>
-      <c r="J37" s="47">
+      <c r="J37" s="46">
         <f t="shared" si="5"/>
         <v>99.043049563810271</v>
       </c>
-      <c r="K37" s="47">
+      <c r="K37" s="46">
         <f t="shared" si="6"/>
         <v>52.229201760000002</v>
       </c>
-      <c r="L37" s="47">
+      <c r="L37" s="46">
         <f t="shared" si="7"/>
         <v>46.813847803810269</v>
       </c>
@@ -7520,10 +7508,10 @@
       <c r="O37" s="27">
         <v>5.6366754364629776E-2</v>
       </c>
-      <c r="P37" s="44">
+      <c r="P37" s="43">
         <v>2.5</v>
       </c>
-      <c r="Q37" s="42">
+      <c r="Q37" s="41">
         <v>6.0392103392567247</v>
       </c>
     </row>

</xml_diff>